<commit_message>
final turn in vers
</commit_message>
<xml_diff>
--- a/testing/scratch work2.xlsx
+++ b/testing/scratch work2.xlsx
@@ -1,19 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27726"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27830"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\panze\PycharmProjects\WSN_HW_1\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\panze\PycharmProjects\WSN_HW_1\testing\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F3235023-813B-40E0-B097-9D1C9D67C171}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CCC0E844-D77B-4984-B8A8-EC479EF5C8BC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="19200" yWindow="0" windowWidth="19200" windowHeight="21000" xr2:uid="{A8A72211-907D-420D-B034-943A9724D965}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="21000" activeTab="1" xr2:uid="{A8A72211-907D-420D-B034-943A9724D965}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$B$19:$I$110</definedName>
@@ -39,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="22">
   <si>
     <t>x</t>
   </si>
@@ -88,6 +89,24 @@
   <si>
     <t>Self</t>
   </si>
+  <si>
+    <t>D</t>
+  </si>
+  <si>
+    <t>f</t>
+  </si>
+  <si>
+    <t>p</t>
+  </si>
+  <si>
+    <t>e</t>
+  </si>
+  <si>
+    <t>r</t>
+  </si>
+  <si>
+    <t>center</t>
+  </si>
 </sst>
 </file>
 
@@ -316,7 +335,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
@@ -337,18 +356,6 @@
     <xf numFmtId="49" fontId="0" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -358,31 +365,32 @@
     <xf numFmtId="49" fontId="0" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="21">
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00B050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF92D050"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="4">
     <dxf>
       <font>
         <color auto="1"/>
@@ -394,132 +402,9 @@
       </fill>
     </dxf>
     <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00B050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
       <fill>
         <patternFill>
           <bgColor rgb="FF92D050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color auto="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00B0F0"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00B050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00B050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF92D050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF92D050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color auto="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00B0F0"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00B050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00B050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF92D050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF92D050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color auto="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00B0F0"/>
         </patternFill>
       </fill>
     </dxf>
@@ -872,7 +757,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{516A8345-3595-4F8B-9771-3F595A41F85F}">
   <dimension ref="B1:L110"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
+    <sheetView topLeftCell="A2" workbookViewId="0">
       <selection activeCell="M30" sqref="M30"/>
     </sheetView>
   </sheetViews>
@@ -880,12 +765,12 @@
   <sheetData>
     <row r="1" spans="2:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="2" spans="2:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D2" s="12" t="s">
+      <c r="D2" s="8" t="s">
         <v>0</v>
       </c>
-      <c r="E2" s="13"/>
-      <c r="F2" s="13"/>
-      <c r="G2" s="14"/>
+      <c r="E2" s="9"/>
+      <c r="F2" s="9"/>
+      <c r="G2" s="10"/>
     </row>
     <row r="3" spans="2:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C3" s="3"/>
@@ -915,110 +800,110 @@
       </c>
     </row>
     <row r="4" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B4" s="10" t="s">
+      <c r="B4" s="11" t="s">
         <v>1</v>
       </c>
-      <c r="C4" s="16" t="s">
+      <c r="C4" s="14" t="s">
         <v>3</v>
       </c>
-      <c r="D4" s="10">
+      <c r="D4" s="11">
         <v>1</v>
       </c>
-      <c r="E4" s="10">
+      <c r="E4" s="11">
         <v>2</v>
       </c>
-      <c r="F4" s="10">
+      <c r="F4" s="11">
         <v>3</v>
       </c>
-      <c r="G4" s="10">
+      <c r="G4" s="11">
         <v>4</v>
       </c>
     </row>
     <row r="5" spans="2:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B5" s="15"/>
-      <c r="C5" s="8"/>
-      <c r="D5" s="11"/>
-      <c r="E5" s="11"/>
-      <c r="F5" s="11"/>
-      <c r="G5" s="11"/>
+      <c r="B5" s="12"/>
+      <c r="C5" s="15"/>
+      <c r="D5" s="13"/>
+      <c r="E5" s="13"/>
+      <c r="F5" s="13"/>
+      <c r="G5" s="13"/>
     </row>
     <row r="6" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B6" s="15"/>
-      <c r="C6" s="8" t="s">
+      <c r="B6" s="12"/>
+      <c r="C6" s="15" t="s">
         <v>5</v>
       </c>
-      <c r="D6" s="10">
+      <c r="D6" s="11">
         <v>5</v>
       </c>
-      <c r="E6" s="10">
+      <c r="E6" s="11">
         <v>6</v>
       </c>
-      <c r="F6" s="10">
+      <c r="F6" s="11">
         <v>7</v>
       </c>
-      <c r="G6" s="10">
+      <c r="G6" s="11">
         <v>8</v>
       </c>
     </row>
     <row r="7" spans="2:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B7" s="15"/>
-      <c r="C7" s="8"/>
-      <c r="D7" s="11"/>
-      <c r="E7" s="11"/>
-      <c r="F7" s="11"/>
-      <c r="G7" s="11"/>
+      <c r="B7" s="12"/>
+      <c r="C7" s="15"/>
+      <c r="D7" s="13"/>
+      <c r="E7" s="13"/>
+      <c r="F7" s="13"/>
+      <c r="G7" s="13"/>
     </row>
     <row r="8" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B8" s="15"/>
-      <c r="C8" s="8" t="s">
+      <c r="B8" s="12"/>
+      <c r="C8" s="15" t="s">
         <v>6</v>
       </c>
-      <c r="D8" s="10">
+      <c r="D8" s="11">
         <v>9</v>
       </c>
-      <c r="E8" s="10">
+      <c r="E8" s="11">
         <v>10</v>
       </c>
-      <c r="F8" s="10">
+      <c r="F8" s="11">
         <v>11</v>
       </c>
-      <c r="G8" s="10">
+      <c r="G8" s="11">
         <v>12</v>
       </c>
     </row>
     <row r="9" spans="2:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B9" s="15"/>
-      <c r="C9" s="8"/>
-      <c r="D9" s="11"/>
-      <c r="E9" s="11"/>
-      <c r="F9" s="11"/>
-      <c r="G9" s="11"/>
+      <c r="B9" s="12"/>
+      <c r="C9" s="15"/>
+      <c r="D9" s="13"/>
+      <c r="E9" s="13"/>
+      <c r="F9" s="13"/>
+      <c r="G9" s="13"/>
     </row>
     <row r="10" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B10" s="15"/>
-      <c r="C10" s="8" t="s">
+      <c r="B10" s="12"/>
+      <c r="C10" s="15" t="s">
         <v>4</v>
       </c>
-      <c r="D10" s="10">
+      <c r="D10" s="11">
         <v>13</v>
       </c>
-      <c r="E10" s="10">
+      <c r="E10" s="11">
         <v>14</v>
       </c>
-      <c r="F10" s="10">
+      <c r="F10" s="11">
         <v>15</v>
       </c>
-      <c r="G10" s="10">
+      <c r="G10" s="11">
         <v>16</v>
       </c>
     </row>
     <row r="11" spans="2:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B11" s="11"/>
-      <c r="C11" s="9"/>
-      <c r="D11" s="11"/>
-      <c r="E11" s="11"/>
-      <c r="F11" s="11"/>
-      <c r="G11" s="11"/>
+      <c r="B11" s="13"/>
+      <c r="C11" s="16"/>
+      <c r="D11" s="13"/>
+      <c r="E11" s="13"/>
+      <c r="F11" s="13"/>
+      <c r="G11" s="13"/>
     </row>
     <row r="14" spans="2:12" x14ac:dyDescent="0.25">
       <c r="C14" s="1" t="s">
@@ -1120,22 +1005,22 @@
         <v>19.04</v>
       </c>
       <c r="E20" s="6">
-        <f>SQRT(($C20 - $D$15)^2 + ($D20 - $E$15)^2)</f>
+        <f t="shared" ref="E20:E51" si="0">SQRT(($C20 - $D$15)^2 + ($D20 - $E$15)^2)</f>
         <v>13.372583893922668</v>
       </c>
       <c r="F20" s="6">
-        <f>SQRT(($C20 - $D$17)^2 + ($D20 - $E$17)^2)</f>
+        <f t="shared" ref="F20:F51" si="1">SQRT(($C20 - $D$17)^2 + ($D20 - $E$17)^2)</f>
         <v>18.047431950280348</v>
       </c>
       <c r="G20" s="1">
         <v>7.99</v>
       </c>
       <c r="H20" s="6" t="str">
-        <f>IF($F$15-$E20&gt;0,"in range","short")</f>
+        <f t="shared" ref="H20:H51" si="2">IF($F$15-$E20&gt;0,"in range","short")</f>
         <v>short</v>
       </c>
       <c r="I20" s="2" t="str">
-        <f>IF(B20=$C$15,"Self",IF(B20=$C$17,"Dest",""))</f>
+        <f t="shared" ref="I20:I51" si="3">IF(B20=$C$15,"Self",IF(B20=$C$17,"Dest",""))</f>
         <v/>
       </c>
     </row>
@@ -1150,22 +1035,22 @@
         <v>17.37</v>
       </c>
       <c r="E21" s="6">
-        <f>SQRT(($C21 - $D$15)^2 + ($D21 - $E$15)^2)</f>
+        <f t="shared" si="0"/>
         <v>12.854143300897187</v>
       </c>
       <c r="F21" s="6">
-        <f>SQRT(($C21 - $D$17)^2 + ($D21 - $E$17)^2)</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="G21" s="1">
         <v>2.58</v>
       </c>
       <c r="H21" s="6" t="str">
-        <f>IF($F$15-$E21&gt;0,"in range","short")</f>
+        <f t="shared" si="2"/>
         <v>short</v>
       </c>
       <c r="I21" s="2" t="str">
-        <f>IF(B21=$C$15,"Self",IF(B21=$C$17,"Dest",""))</f>
+        <f t="shared" si="3"/>
         <v>Dest</v>
       </c>
     </row>
@@ -1180,22 +1065,22 @@
         <v>19.36</v>
       </c>
       <c r="E22" s="6">
-        <f>SQRT(($C22 - $D$15)^2 + ($D22 - $E$15)^2)</f>
+        <f t="shared" si="0"/>
         <v>13.074421593324884</v>
       </c>
       <c r="F22" s="6">
-        <f>SQRT(($C22 - $D$17)^2 + ($D22 - $E$17)^2)</f>
+        <f t="shared" si="1"/>
         <v>17.175671748144232</v>
       </c>
       <c r="G22" s="1">
         <v>2</v>
       </c>
       <c r="H22" s="6" t="str">
-        <f>IF($F$15-$E22&gt;0,"in range","short")</f>
+        <f t="shared" si="2"/>
         <v>short</v>
       </c>
       <c r="I22" s="2" t="str">
-        <f>IF(B22=$C$15,"Self",IF(B22=$C$17,"Dest",""))</f>
+        <f t="shared" si="3"/>
         <v/>
       </c>
     </row>
@@ -1210,22 +1095,22 @@
         <v>17.47</v>
       </c>
       <c r="E23" s="6">
-        <f>SQRT(($C23 - $D$15)^2 + ($D23 - $E$15)^2)</f>
+        <f t="shared" si="0"/>
         <v>9.4725550935320513</v>
       </c>
       <c r="F23" s="6">
-        <f>SQRT(($C23 - $D$17)^2 + ($D23 - $E$17)^2)</f>
+        <f t="shared" si="1"/>
         <v>13.070382549872058</v>
       </c>
       <c r="G23" s="1">
         <v>7.59</v>
       </c>
       <c r="H23" s="6" t="str">
-        <f>IF($F$15-$E23&gt;0,"in range","short")</f>
+        <f t="shared" si="2"/>
         <v>short</v>
       </c>
       <c r="I23" s="2" t="str">
-        <f>IF(B23=$C$15,"Self",IF(B23=$C$17,"Dest",""))</f>
+        <f t="shared" si="3"/>
         <v/>
       </c>
     </row>
@@ -1240,22 +1125,22 @@
         <v>18.71</v>
       </c>
       <c r="E24" s="6">
-        <f>SQRT(($C24 - $D$15)^2 + ($D24 - $E$15)^2)</f>
+        <f t="shared" si="0"/>
         <v>13.301793112208596</v>
       </c>
       <c r="F24" s="6">
-        <f>SQRT(($C24 - $D$17)^2 + ($D24 - $E$17)^2)</f>
+        <f t="shared" si="1"/>
         <v>1.5259423318068084</v>
       </c>
       <c r="G24" s="1">
         <v>2.38</v>
       </c>
       <c r="H24" s="6" t="str">
-        <f>IF($F$15-$E24&gt;0,"in range","short")</f>
+        <f t="shared" si="2"/>
         <v>short</v>
       </c>
       <c r="I24" s="2" t="str">
-        <f>IF(B24=$C$15,"Self",IF(B24=$C$17,"Dest",""))</f>
+        <f t="shared" si="3"/>
         <v/>
       </c>
     </row>
@@ -1270,22 +1155,22 @@
         <v>17.93</v>
       </c>
       <c r="E25" s="6">
-        <f>SQRT(($C25 - $D$15)^2 + ($D25 - $E$15)^2)</f>
+        <f t="shared" si="0"/>
         <v>11.266077400763763</v>
       </c>
       <c r="F25" s="6">
-        <f>SQRT(($C25 - $D$17)^2 + ($D25 - $E$17)^2)</f>
+        <f t="shared" si="1"/>
         <v>15.959827693305463</v>
       </c>
       <c r="G25" s="1">
         <v>2.14</v>
       </c>
       <c r="H25" s="6" t="str">
-        <f>IF($F$15-$E25&gt;0,"in range","short")</f>
+        <f t="shared" si="2"/>
         <v>short</v>
       </c>
       <c r="I25" s="2" t="str">
-        <f>IF(B25=$C$15,"Self",IF(B25=$C$17,"Dest",""))</f>
+        <f t="shared" si="3"/>
         <v/>
       </c>
     </row>
@@ -1300,22 +1185,22 @@
         <v>15.46</v>
       </c>
       <c r="E26" s="6">
-        <f>SQRT(($C26 - $D$15)^2 + ($D26 - $E$15)^2)</f>
+        <f t="shared" si="0"/>
         <v>9.9933577940550098</v>
       </c>
       <c r="F26" s="6">
-        <f>SQRT(($C26 - $D$17)^2 + ($D26 - $E$17)^2)</f>
+        <f t="shared" si="1"/>
         <v>2.8609439001839938</v>
       </c>
       <c r="G26" s="1">
         <v>4.26</v>
       </c>
       <c r="H26" s="6" t="str">
-        <f>IF($F$15-$E26&gt;0,"in range","short")</f>
+        <f t="shared" si="2"/>
         <v>short</v>
       </c>
       <c r="I26" s="2" t="str">
-        <f>IF(B26=$C$15,"Self",IF(B26=$C$17,"Dest",""))</f>
+        <f t="shared" si="3"/>
         <v/>
       </c>
     </row>
@@ -1330,22 +1215,22 @@
         <v>18.63</v>
       </c>
       <c r="E27" s="6">
-        <f>SQRT(($C27 - $D$15)^2 + ($D27 - $E$15)^2)</f>
+        <f t="shared" si="0"/>
         <v>11.560765545585637</v>
       </c>
       <c r="F27" s="6">
-        <f>SQRT(($C27 - $D$17)^2 + ($D27 - $E$17)^2)</f>
+        <f t="shared" si="1"/>
         <v>15.461426195535779</v>
       </c>
       <c r="G27" s="1">
         <v>7.92</v>
       </c>
       <c r="H27" s="6" t="str">
-        <f>IF($F$15-$E27&gt;0,"in range","short")</f>
+        <f t="shared" si="2"/>
         <v>short</v>
       </c>
       <c r="I27" s="2" t="str">
-        <f>IF(B27=$C$15,"Self",IF(B27=$C$17,"Dest",""))</f>
+        <f t="shared" si="3"/>
         <v/>
       </c>
     </row>
@@ -1360,22 +1245,22 @@
         <v>3.18</v>
       </c>
       <c r="E28" s="6">
-        <f>SQRT(($C28 - $D$15)^2 + ($D28 - $E$15)^2)</f>
+        <f t="shared" si="0"/>
         <v>9.5556475447768587</v>
       </c>
       <c r="F28" s="6">
-        <f>SQRT(($C28 - $D$17)^2 + ($D28 - $E$17)^2)</f>
+        <f t="shared" si="1"/>
         <v>14.290283412165065</v>
       </c>
       <c r="G28" s="1">
         <v>7.7</v>
       </c>
       <c r="H28" s="6" t="str">
-        <f>IF($F$15-$E28&gt;0,"in range","short")</f>
+        <f t="shared" si="2"/>
         <v>short</v>
       </c>
       <c r="I28" s="2" t="str">
-        <f>IF(B28=$C$15,"Self",IF(B28=$C$17,"Dest",""))</f>
+        <f t="shared" si="3"/>
         <v/>
       </c>
     </row>
@@ -1390,22 +1275,22 @@
         <v>19.66</v>
       </c>
       <c r="E29" s="6">
-        <f>SQRT(($C29 - $D$15)^2 + ($D29 - $E$15)^2)</f>
+        <f t="shared" si="0"/>
         <v>12.940479125596548</v>
       </c>
       <c r="F29" s="6">
-        <f>SQRT(($C29 - $D$17)^2 + ($D29 - $E$17)^2)</f>
+        <f t="shared" si="1"/>
         <v>3.4722039110628278</v>
       </c>
       <c r="G29" s="1">
         <v>3.87</v>
       </c>
       <c r="H29" s="6" t="str">
-        <f>IF($F$15-$E29&gt;0,"in range","short")</f>
+        <f t="shared" si="2"/>
         <v>short</v>
       </c>
       <c r="I29" s="2" t="str">
-        <f>IF(B29=$C$15,"Self",IF(B29=$C$17,"Dest",""))</f>
+        <f t="shared" si="3"/>
         <v/>
       </c>
     </row>
@@ -1420,22 +1305,22 @@
         <v>15.87</v>
       </c>
       <c r="E30" s="6">
-        <f>SQRT(($C30 - $D$15)^2 + ($D30 - $E$15)^2)</f>
+        <f t="shared" si="0"/>
         <v>9.8817457971757197</v>
       </c>
       <c r="F30" s="6">
-        <f>SQRT(($C30 - $D$17)^2 + ($D30 - $E$17)^2)</f>
+        <f t="shared" si="1"/>
         <v>16.358915000696101</v>
       </c>
       <c r="G30" s="1">
         <v>2.17</v>
       </c>
       <c r="H30" s="6" t="str">
-        <f>IF($F$15-$E30&gt;0,"in range","short")</f>
+        <f t="shared" si="2"/>
         <v>short</v>
       </c>
       <c r="I30" s="2" t="str">
-        <f>IF(B30=$C$15,"Self",IF(B30=$C$17,"Dest",""))</f>
+        <f t="shared" si="3"/>
         <v/>
       </c>
     </row>
@@ -1450,22 +1335,22 @@
         <v>18.55</v>
       </c>
       <c r="E31" s="6">
-        <f>SQRT(($C31 - $D$15)^2 + ($D31 - $E$15)^2)</f>
+        <f t="shared" si="0"/>
         <v>10.719860073713649</v>
       </c>
       <c r="F31" s="6">
-        <f>SQRT(($C31 - $D$17)^2 + ($D31 - $E$17)^2)</f>
+        <f t="shared" si="1"/>
         <v>13.770649948350295</v>
       </c>
       <c r="G31" s="1">
         <v>4.24</v>
       </c>
       <c r="H31" s="6" t="str">
-        <f>IF($F$15-$E31&gt;0,"in range","short")</f>
+        <f t="shared" si="2"/>
         <v>short</v>
       </c>
       <c r="I31" s="2" t="str">
-        <f>IF(B31=$C$15,"Self",IF(B31=$C$17,"Dest",""))</f>
+        <f t="shared" si="3"/>
         <v/>
       </c>
     </row>
@@ -1480,22 +1365,22 @@
         <v>15.17</v>
       </c>
       <c r="E32" s="6">
-        <f>SQRT(($C32 - $D$15)^2 + ($D32 - $E$15)^2)</f>
+        <f t="shared" si="0"/>
         <v>9.065506053166585</v>
       </c>
       <c r="F32" s="6">
-        <f>SQRT(($C32 - $D$17)^2 + ($D32 - $E$17)^2)</f>
+        <f t="shared" si="1"/>
         <v>3.8340057381282051</v>
       </c>
       <c r="G32" s="1">
         <v>7.5</v>
       </c>
       <c r="H32" s="6" t="str">
-        <f>IF($F$15-$E32&gt;0,"in range","short")</f>
+        <f t="shared" si="2"/>
         <v>short</v>
       </c>
       <c r="I32" s="2" t="str">
-        <f>IF(B32=$C$15,"Self",IF(B32=$C$17,"Dest",""))</f>
+        <f t="shared" si="3"/>
         <v/>
       </c>
     </row>
@@ -1510,22 +1395,22 @@
         <v>13.6</v>
       </c>
       <c r="E33" s="6">
-        <f>SQRT(($C33 - $D$15)^2 + ($D33 - $E$15)^2)</f>
+        <f t="shared" si="0"/>
         <v>8.1240630228968556</v>
       </c>
       <c r="F33" s="6">
-        <f>SQRT(($C33 - $D$17)^2 + ($D33 - $E$17)^2)</f>
+        <f t="shared" si="1"/>
         <v>16.408954872264108</v>
       </c>
       <c r="G33" s="1">
         <v>5.54</v>
       </c>
       <c r="H33" s="6" t="str">
-        <f>IF($F$15-$E33&gt;0,"in range","short")</f>
+        <f t="shared" si="2"/>
         <v>short</v>
       </c>
       <c r="I33" s="2" t="str">
-        <f>IF(B33=$C$15,"Self",IF(B33=$C$17,"Dest",""))</f>
+        <f t="shared" si="3"/>
         <v/>
       </c>
     </row>
@@ -1540,22 +1425,22 @@
         <v>18.93</v>
       </c>
       <c r="E34" s="6">
-        <f>SQRT(($C34 - $D$15)^2 + ($D34 - $E$15)^2)</f>
+        <f t="shared" si="0"/>
         <v>10.496447017919921</v>
       </c>
       <c r="F34" s="6">
-        <f>SQRT(($C34 - $D$17)^2 + ($D34 - $E$17)^2)</f>
+        <f t="shared" si="1"/>
         <v>11.94232808124111</v>
       </c>
       <c r="G34" s="1">
         <v>4.0599999999999996</v>
       </c>
       <c r="H34" s="6" t="str">
-        <f>IF($F$15-$E34&gt;0,"in range","short")</f>
+        <f t="shared" si="2"/>
         <v>short</v>
       </c>
       <c r="I34" s="2" t="str">
-        <f>IF(B34=$C$15,"Self",IF(B34=$C$17,"Dest",""))</f>
+        <f t="shared" si="3"/>
         <v/>
       </c>
     </row>
@@ -1570,22 +1455,22 @@
         <v>18.04</v>
       </c>
       <c r="E35" s="6">
-        <f>SQRT(($C35 - $D$15)^2 + ($D35 - $E$15)^2)</f>
+        <f t="shared" si="0"/>
         <v>10.469407815153634</v>
       </c>
       <c r="F35" s="6">
-        <f>SQRT(($C35 - $D$17)^2 + ($D35 - $E$17)^2)</f>
+        <f t="shared" si="1"/>
         <v>4.8069220921500273</v>
       </c>
       <c r="G35" s="1">
         <v>6.77</v>
       </c>
       <c r="H35" s="6" t="str">
-        <f>IF($F$15-$E35&gt;0,"in range","short")</f>
+        <f t="shared" si="2"/>
         <v>short</v>
       </c>
       <c r="I35" s="2" t="str">
-        <f>IF(B35=$C$15,"Self",IF(B35=$C$17,"Dest",""))</f>
+        <f t="shared" si="3"/>
         <v/>
       </c>
     </row>
@@ -1600,22 +1485,22 @@
         <v>14.06</v>
       </c>
       <c r="E36" s="6">
-        <f>SQRT(($C36 - $D$15)^2 + ($D36 - $E$15)^2)</f>
+        <f t="shared" si="0"/>
         <v>7.6298427244603158</v>
       </c>
       <c r="F36" s="6">
-        <f>SQRT(($C36 - $D$17)^2 + ($D36 - $E$17)^2)</f>
+        <f t="shared" si="1"/>
         <v>5.2382917062721885</v>
       </c>
       <c r="G36" s="1">
         <v>5.24</v>
       </c>
       <c r="H36" s="6" t="str">
-        <f>IF($F$15-$E36&gt;0,"in range","short")</f>
+        <f t="shared" si="2"/>
         <v>short</v>
       </c>
       <c r="I36" s="2" t="str">
-        <f>IF(B36=$C$15,"Self",IF(B36=$C$17,"Dest",""))</f>
+        <f t="shared" si="3"/>
         <v/>
       </c>
     </row>
@@ -1630,22 +1515,22 @@
         <v>17.86</v>
       </c>
       <c r="E37" s="6">
-        <f>SQRT(($C37 - $D$15)^2 + ($D37 - $E$15)^2)</f>
+        <f t="shared" si="0"/>
         <v>10.048009753179981</v>
       </c>
       <c r="F37" s="6">
-        <f>SQRT(($C37 - $D$17)^2 + ($D37 - $E$17)^2)</f>
+        <f t="shared" si="1"/>
         <v>5.3823507875276944</v>
       </c>
       <c r="G37" s="1">
         <v>2.5499999999999998</v>
       </c>
       <c r="H37" s="6" t="str">
-        <f>IF($F$15-$E37&gt;0,"in range","short")</f>
+        <f t="shared" si="2"/>
         <v>short</v>
       </c>
       <c r="I37" s="2" t="str">
-        <f>IF(B37=$C$15,"Self",IF(B37=$C$17,"Dest",""))</f>
+        <f t="shared" si="3"/>
         <v/>
       </c>
     </row>
@@ -1660,22 +1545,22 @@
         <v>12.19</v>
       </c>
       <c r="E38" s="6">
-        <f>SQRT(($C38 - $D$15)^2 + ($D38 - $E$15)^2)</f>
+        <f t="shared" si="0"/>
         <v>8.1726495091861135</v>
       </c>
       <c r="F38" s="6">
-        <f>SQRT(($C38 - $D$17)^2 + ($D38 - $E$17)^2)</f>
+        <f t="shared" si="1"/>
         <v>5.5894901377495971</v>
       </c>
       <c r="G38" s="1">
         <v>5.17</v>
       </c>
       <c r="H38" s="6" t="str">
-        <f>IF($F$15-$E38&gt;0,"in range","short")</f>
+        <f t="shared" si="2"/>
         <v>short</v>
       </c>
       <c r="I38" s="2" t="str">
-        <f>IF(B38=$C$15,"Self",IF(B38=$C$17,"Dest",""))</f>
+        <f t="shared" si="3"/>
         <v/>
       </c>
     </row>
@@ -1690,22 +1575,22 @@
         <v>19.12</v>
       </c>
       <c r="E39" s="6">
-        <f>SQRT(($C39 - $D$15)^2 + ($D39 - $E$15)^2)</f>
+        <f t="shared" si="0"/>
         <v>11.118938798284665</v>
       </c>
       <c r="F39" s="6">
-        <f>SQRT(($C39 - $D$17)^2 + ($D39 - $E$17)^2)</f>
+        <f t="shared" si="1"/>
         <v>5.8766146717306551</v>
       </c>
       <c r="G39" s="1">
         <v>3.87</v>
       </c>
       <c r="H39" s="6" t="str">
-        <f>IF($F$15-$E39&gt;0,"in range","short")</f>
+        <f t="shared" si="2"/>
         <v>short</v>
       </c>
       <c r="I39" s="2" t="str">
-        <f>IF(B39=$C$15,"Self",IF(B39=$C$17,"Dest",""))</f>
+        <f t="shared" si="3"/>
         <v/>
       </c>
     </row>
@@ -1720,22 +1605,22 @@
         <v>12.82</v>
       </c>
       <c r="E40" s="6">
-        <f>SQRT(($C40 - $D$15)^2 + ($D40 - $E$15)^2)</f>
+        <f t="shared" si="0"/>
         <v>8.3128093927384157</v>
       </c>
       <c r="F40" s="6">
-        <f>SQRT(($C40 - $D$17)^2 + ($D40 - $E$17)^2)</f>
+        <f t="shared" si="1"/>
         <v>17.318389070580441</v>
       </c>
       <c r="G40" s="1">
         <v>1.62</v>
       </c>
       <c r="H40" s="6" t="str">
-        <f>IF($F$15-$E40&gt;0,"in range","short")</f>
+        <f t="shared" si="2"/>
         <v>short</v>
       </c>
       <c r="I40" s="2" t="str">
-        <f>IF(B40=$C$15,"Self",IF(B40=$C$17,"Dest",""))</f>
+        <f t="shared" si="3"/>
         <v/>
       </c>
     </row>
@@ -1750,22 +1635,22 @@
         <v>13.35</v>
       </c>
       <c r="E41" s="6">
-        <f>SQRT(($C41 - $D$15)^2 + ($D41 - $E$15)^2)</f>
+        <f t="shared" si="0"/>
         <v>6.4500697670645399</v>
       </c>
       <c r="F41" s="6">
-        <f>SQRT(($C41 - $D$17)^2 + ($D41 - $E$17)^2)</f>
+        <f t="shared" si="1"/>
         <v>6.4312362730660118</v>
       </c>
       <c r="G41" s="1">
         <v>7.22</v>
       </c>
       <c r="H41" s="6" t="str">
-        <f>IF($F$15-$E41&gt;0,"in range","short")</f>
+        <f t="shared" si="2"/>
         <v>in range</v>
       </c>
       <c r="I41" s="2" t="str">
-        <f>IF(B41=$C$15,"Self",IF(B41=$C$17,"Dest",""))</f>
+        <f t="shared" si="3"/>
         <v/>
       </c>
     </row>
@@ -1780,22 +1665,22 @@
         <v>11.13</v>
       </c>
       <c r="E42" s="6">
-        <f>SQRT(($C42 - $D$15)^2 + ($D42 - $E$15)^2)</f>
+        <f t="shared" si="0"/>
         <v>7.2117265616494368</v>
       </c>
       <c r="F42" s="6">
-        <f>SQRT(($C42 - $D$17)^2 + ($D42 - $E$17)^2)</f>
+        <f t="shared" si="1"/>
         <v>6.7990881741598264</v>
       </c>
       <c r="G42" s="1">
         <v>6.96</v>
       </c>
       <c r="H42" s="6" t="str">
-        <f>IF($F$15-$E42&gt;0,"in range","short")</f>
+        <f t="shared" si="2"/>
         <v>in range</v>
       </c>
       <c r="I42" s="2" t="str">
-        <f>IF(B42=$C$15,"Self",IF(B42=$C$17,"Dest",""))</f>
+        <f t="shared" si="3"/>
         <v/>
       </c>
     </row>
@@ -1810,22 +1695,22 @@
         <v>11.24</v>
       </c>
       <c r="E43" s="6">
-        <f>SQRT(($C43 - $D$15)^2 + ($D43 - $E$15)^2)</f>
+        <f t="shared" si="0"/>
         <v>6.5892336428449712</v>
       </c>
       <c r="F43" s="6">
-        <f>SQRT(($C43 - $D$17)^2 + ($D43 - $E$17)^2)</f>
+        <f t="shared" si="1"/>
         <v>7.0146275738630637</v>
       </c>
       <c r="G43" s="1">
         <v>2.8</v>
       </c>
       <c r="H43" s="6" t="str">
-        <f>IF($F$15-$E43&gt;0,"in range","short")</f>
+        <f t="shared" si="2"/>
         <v>in range</v>
       </c>
       <c r="I43" s="2" t="str">
-        <f>IF(B43=$C$15,"Self",IF(B43=$C$17,"Dest",""))</f>
+        <f t="shared" si="3"/>
         <v/>
       </c>
     </row>
@@ -1840,22 +1725,22 @@
         <v>17.23</v>
       </c>
       <c r="E44" s="6">
-        <f>SQRT(($C44 - $D$15)^2 + ($D44 - $E$15)^2)</f>
+        <f t="shared" si="0"/>
         <v>8.8776404522823533</v>
       </c>
       <c r="F44" s="6">
-        <f>SQRT(($C44 - $D$17)^2 + ($D44 - $E$17)^2)</f>
+        <f t="shared" si="1"/>
         <v>7.0313938874166331</v>
       </c>
       <c r="G44" s="1">
         <v>1.95</v>
       </c>
       <c r="H44" s="6" t="str">
-        <f>IF($F$15-$E44&gt;0,"in range","short")</f>
+        <f t="shared" si="2"/>
         <v>short</v>
       </c>
       <c r="I44" s="2" t="str">
-        <f>IF(B44=$C$15,"Self",IF(B44=$C$17,"Dest",""))</f>
+        <f t="shared" si="3"/>
         <v/>
       </c>
     </row>
@@ -1870,22 +1755,22 @@
         <v>12.63</v>
       </c>
       <c r="E45" s="6">
-        <f>SQRT(($C45 - $D$15)^2 + ($D45 - $E$15)^2)</f>
+        <f t="shared" si="0"/>
         <v>8.7788040187715772</v>
       </c>
       <c r="F45" s="6">
-        <f>SQRT(($C45 - $D$17)^2 + ($D45 - $E$17)^2)</f>
+        <f t="shared" si="1"/>
         <v>17.976184244716674</v>
       </c>
       <c r="G45" s="1">
         <v>7.09</v>
       </c>
       <c r="H45" s="6" t="str">
-        <f>IF($F$15-$E45&gt;0,"in range","short")</f>
+        <f t="shared" si="2"/>
         <v>short</v>
       </c>
       <c r="I45" s="2" t="str">
-        <f>IF(B45=$C$15,"Self",IF(B45=$C$17,"Dest",""))</f>
+        <f t="shared" si="3"/>
         <v/>
       </c>
     </row>
@@ -1900,22 +1785,22 @@
         <v>14.35</v>
       </c>
       <c r="E46" s="6">
-        <f>SQRT(($C46 - $D$15)^2 + ($D46 - $E$15)^2)</f>
+        <f t="shared" si="0"/>
         <v>6.4445713589035547</v>
       </c>
       <c r="F46" s="6">
-        <f>SQRT(($C46 - $D$17)^2 + ($D46 - $E$17)^2)</f>
+        <f t="shared" si="1"/>
         <v>7.0677082565708673</v>
       </c>
       <c r="G46" s="1">
         <v>2.66</v>
       </c>
       <c r="H46" s="6" t="str">
-        <f>IF($F$15-$E46&gt;0,"in range","short")</f>
+        <f t="shared" si="2"/>
         <v>in range</v>
       </c>
       <c r="I46" s="2" t="str">
-        <f>IF(B46=$C$15,"Self",IF(B46=$C$17,"Dest",""))</f>
+        <f t="shared" si="3"/>
         <v/>
       </c>
     </row>
@@ -1930,22 +1815,22 @@
         <v>12.61</v>
       </c>
       <c r="E47" s="6">
-        <f>SQRT(($C47 - $D$15)^2 + ($D47 - $E$15)^2)</f>
+        <f t="shared" si="0"/>
         <v>5.6078962187258785</v>
       </c>
       <c r="F47" s="6">
-        <f>SQRT(($C47 - $D$17)^2 + ($D47 - $E$17)^2)</f>
+        <f t="shared" si="1"/>
         <v>7.251103364316358</v>
       </c>
       <c r="G47" s="1">
         <v>6.38</v>
       </c>
       <c r="H47" s="6" t="str">
-        <f>IF($F$15-$E47&gt;0,"in range","short")</f>
+        <f t="shared" si="2"/>
         <v>in range</v>
       </c>
       <c r="I47" s="2" t="str">
-        <f>IF(B47=$C$15,"Self",IF(B47=$C$17,"Dest",""))</f>
+        <f t="shared" si="3"/>
         <v/>
       </c>
     </row>
@@ -1960,22 +1845,22 @@
         <v>10.27</v>
       </c>
       <c r="E48" s="6">
-        <f>SQRT(($C48 - $D$15)^2 + ($D48 - $E$15)^2)</f>
+        <f t="shared" si="0"/>
         <v>7.8094430019048096</v>
       </c>
       <c r="F48" s="6">
-        <f>SQRT(($C48 - $D$17)^2 + ($D48 - $E$17)^2)</f>
+        <f t="shared" si="1"/>
         <v>7.3345483841883556</v>
       </c>
       <c r="G48" s="1">
         <v>7.36</v>
       </c>
       <c r="H48" s="6" t="str">
-        <f>IF($F$15-$E48&gt;0,"in range","short")</f>
+        <f t="shared" si="2"/>
         <v>short</v>
       </c>
       <c r="I48" s="2" t="str">
-        <f>IF(B48=$C$15,"Self",IF(B48=$C$17,"Dest",""))</f>
+        <f t="shared" si="3"/>
         <v/>
       </c>
     </row>
@@ -1990,22 +1875,22 @@
         <v>10.26</v>
       </c>
       <c r="E49" s="6">
-        <f>SQRT(($C49 - $D$15)^2 + ($D49 - $E$15)^2)</f>
+        <f t="shared" si="0"/>
         <v>6.0544281315414095</v>
       </c>
       <c r="F49" s="6">
-        <f>SQRT(($C49 - $D$17)^2 + ($D49 - $E$17)^2)</f>
+        <f t="shared" si="1"/>
         <v>7.9875966347832073</v>
       </c>
       <c r="G49" s="1">
         <v>4.6900000000000004</v>
       </c>
       <c r="H49" s="6" t="str">
-        <f>IF($F$15-$E49&gt;0,"in range","short")</f>
+        <f t="shared" si="2"/>
         <v>in range</v>
       </c>
       <c r="I49" s="2" t="str">
-        <f>IF(B49=$C$15,"Self",IF(B49=$C$17,"Dest",""))</f>
+        <f t="shared" si="3"/>
         <v/>
       </c>
     </row>
@@ -2020,22 +1905,22 @@
         <v>17.23</v>
       </c>
       <c r="E50" s="6">
-        <f>SQRT(($C50 - $D$15)^2 + ($D50 - $E$15)^2)</f>
+        <f t="shared" si="0"/>
         <v>8.6506936138092438</v>
       </c>
       <c r="F50" s="6">
-        <f>SQRT(($C50 - $D$17)^2 + ($D50 - $E$17)^2)</f>
+        <f t="shared" si="1"/>
         <v>8.0512172992659927</v>
       </c>
       <c r="G50" s="1">
         <v>3.61</v>
       </c>
       <c r="H50" s="6" t="str">
-        <f>IF($F$15-$E50&gt;0,"in range","short")</f>
+        <f t="shared" si="2"/>
         <v>short</v>
       </c>
       <c r="I50" s="2" t="str">
-        <f>IF(B50=$C$15,"Self",IF(B50=$C$17,"Dest",""))</f>
+        <f t="shared" si="3"/>
         <v/>
       </c>
     </row>
@@ -2050,22 +1935,22 @@
         <v>9.83</v>
       </c>
       <c r="E51" s="6">
-        <f>SQRT(($C51 - $D$15)^2 + ($D51 - $E$15)^2)</f>
+        <f t="shared" si="0"/>
         <v>6.2627869195750225</v>
       </c>
       <c r="F51" s="6">
-        <f>SQRT(($C51 - $D$17)^2 + ($D51 - $E$17)^2)</f>
+        <f t="shared" si="1"/>
         <v>8.242602744279262</v>
       </c>
       <c r="G51" s="1">
         <v>5.2</v>
       </c>
       <c r="H51" s="6" t="str">
-        <f>IF($F$15-$E51&gt;0,"in range","short")</f>
+        <f t="shared" si="2"/>
         <v>in range</v>
       </c>
       <c r="I51" s="2" t="str">
-        <f>IF(B51=$C$15,"Self",IF(B51=$C$17,"Dest",""))</f>
+        <f t="shared" si="3"/>
         <v/>
       </c>
     </row>
@@ -2080,22 +1965,22 @@
         <v>18.41</v>
       </c>
       <c r="E52" s="6">
-        <f>SQRT(($C52 - $D$15)^2 + ($D52 - $E$15)^2)</f>
+        <f t="shared" ref="E52:E83" si="4">SQRT(($C52 - $D$15)^2 + ($D52 - $E$15)^2)</f>
         <v>9.7366575373687674</v>
       </c>
       <c r="F52" s="6">
-        <f>SQRT(($C52 - $D$17)^2 + ($D52 - $E$17)^2)</f>
+        <f t="shared" ref="F52:F83" si="5">SQRT(($C52 - $D$17)^2 + ($D52 - $E$17)^2)</f>
         <v>8.8314494846542591</v>
       </c>
       <c r="G52" s="1">
         <v>7.58</v>
       </c>
       <c r="H52" s="6" t="str">
-        <f>IF($F$15-$E52&gt;0,"in range","short")</f>
+        <f t="shared" ref="H52:H83" si="6">IF($F$15-$E52&gt;0,"in range","short")</f>
         <v>short</v>
       </c>
       <c r="I52" s="2" t="str">
-        <f>IF(B52=$C$15,"Self",IF(B52=$C$17,"Dest",""))</f>
+        <f t="shared" ref="I52:I83" si="7">IF(B52=$C$15,"Self",IF(B52=$C$17,"Dest",""))</f>
         <v/>
       </c>
     </row>
@@ -2110,22 +1995,22 @@
         <v>10.220000000000001</v>
       </c>
       <c r="E53" s="6">
-        <f>SQRT(($C53 - $D$15)^2 + ($D53 - $E$15)^2)</f>
+        <f t="shared" si="4"/>
         <v>4.2884146254764142</v>
       </c>
       <c r="F53" s="6">
-        <f>SQRT(($C53 - $D$17)^2 + ($D53 - $E$17)^2)</f>
+        <f t="shared" si="5"/>
         <v>9.0084904395797629</v>
       </c>
       <c r="G53" s="1">
         <v>7.63</v>
       </c>
       <c r="H53" s="6" t="str">
-        <f>IF($F$15-$E53&gt;0,"in range","short")</f>
+        <f t="shared" si="6"/>
         <v>in range</v>
       </c>
       <c r="I53" s="2" t="str">
-        <f>IF(B53=$C$15,"Self",IF(B53=$C$17,"Dest",""))</f>
+        <f t="shared" si="7"/>
         <v/>
       </c>
     </row>
@@ -2140,22 +2025,22 @@
         <v>9.2200000000000006</v>
       </c>
       <c r="E54" s="6">
-        <f>SQRT(($C54 - $D$15)^2 + ($D54 - $E$15)^2)</f>
+        <f t="shared" si="4"/>
         <v>5.3055442699123718</v>
       </c>
       <c r="F54" s="6">
-        <f>SQRT(($C54 - $D$17)^2 + ($D54 - $E$17)^2)</f>
+        <f t="shared" si="5"/>
         <v>9.1731455891640579</v>
       </c>
       <c r="G54" s="1">
         <v>4.28</v>
       </c>
       <c r="H54" s="6" t="str">
-        <f>IF($F$15-$E54&gt;0,"in range","short")</f>
+        <f t="shared" si="6"/>
         <v>in range</v>
       </c>
       <c r="I54" s="2" t="str">
-        <f>IF(B54=$C$15,"Self",IF(B54=$C$17,"Dest",""))</f>
+        <f t="shared" si="7"/>
         <v/>
       </c>
     </row>
@@ -2170,22 +2055,22 @@
         <v>8.14</v>
       </c>
       <c r="E55" s="6">
-        <f>SQRT(($C55 - $D$15)^2 + ($D55 - $E$15)^2)</f>
+        <f t="shared" si="4"/>
         <v>4.8921569884867759</v>
       </c>
       <c r="F55" s="6">
-        <f>SQRT(($C55 - $D$17)^2 + ($D55 - $E$17)^2)</f>
+        <f t="shared" si="5"/>
         <v>10.326170635816551</v>
       </c>
       <c r="G55" s="1">
         <v>2.2200000000000002</v>
       </c>
       <c r="H55" s="6" t="str">
-        <f>IF($F$15-$E55&gt;0,"in range","short")</f>
+        <f t="shared" si="6"/>
         <v>in range</v>
       </c>
       <c r="I55" s="2" t="str">
-        <f>IF(B55=$C$15,"Self",IF(B55=$C$17,"Dest",""))</f>
+        <f t="shared" si="7"/>
         <v/>
       </c>
     </row>
@@ -2200,22 +2085,22 @@
         <v>8.84</v>
       </c>
       <c r="E56" s="6">
-        <f>SQRT(($C56 - $D$15)^2 + ($D56 - $E$15)^2)</f>
+        <f t="shared" si="4"/>
         <v>3.0931698951076072</v>
       </c>
       <c r="F56" s="6">
-        <f>SQRT(($C56 - $D$17)^2 + ($D56 - $E$17)^2)</f>
+        <f t="shared" si="5"/>
         <v>10.664000187546886</v>
       </c>
       <c r="G56" s="1">
         <v>1.74</v>
       </c>
       <c r="H56" s="6" t="str">
-        <f>IF($F$15-$E56&gt;0,"in range","short")</f>
+        <f t="shared" si="6"/>
         <v>in range</v>
       </c>
       <c r="I56" s="2" t="str">
-        <f>IF(B56=$C$15,"Self",IF(B56=$C$17,"Dest",""))</f>
+        <f t="shared" si="7"/>
         <v/>
       </c>
     </row>
@@ -2230,22 +2115,22 @@
         <v>1.42</v>
       </c>
       <c r="E57" s="6">
-        <f>SQRT(($C57 - $D$15)^2 + ($D57 - $E$15)^2)</f>
+        <f t="shared" si="4"/>
         <v>7.5658443018608299</v>
       </c>
       <c r="F57" s="6">
-        <f>SQRT(($C57 - $D$17)^2 + ($D57 - $E$17)^2)</f>
+        <f t="shared" si="5"/>
         <v>17.595664238669709</v>
       </c>
       <c r="G57" s="1">
         <v>6.95</v>
       </c>
       <c r="H57" s="6" t="str">
-        <f>IF($F$15-$E57&gt;0,"in range","short")</f>
+        <f t="shared" si="6"/>
         <v>short</v>
       </c>
       <c r="I57" s="2" t="str">
-        <f>IF(B57=$C$15,"Self",IF(B57=$C$17,"Dest",""))</f>
+        <f t="shared" si="7"/>
         <v/>
       </c>
     </row>
@@ -2260,22 +2145,22 @@
         <v>7.13</v>
       </c>
       <c r="E58" s="6">
-        <f>SQRT(($C58 - $D$15)^2 + ($D58 - $E$15)^2)</f>
+        <f t="shared" si="4"/>
         <v>6.2600718845712953</v>
       </c>
       <c r="F58" s="6">
-        <f>SQRT(($C58 - $D$17)^2 + ($D58 - $E$17)^2)</f>
+        <f t="shared" si="5"/>
         <v>10.799189784423646</v>
       </c>
       <c r="G58" s="1">
         <v>3.77</v>
       </c>
       <c r="H58" s="6" t="str">
-        <f>IF($F$15-$E58&gt;0,"in range","short")</f>
+        <f t="shared" si="6"/>
         <v>in range</v>
       </c>
       <c r="I58" s="2" t="str">
-        <f>IF(B58=$C$15,"Self",IF(B58=$C$17,"Dest",""))</f>
+        <f t="shared" si="7"/>
         <v/>
       </c>
     </row>
@@ -2290,22 +2175,22 @@
         <v>11.3</v>
       </c>
       <c r="E59" s="6">
-        <f>SQRT(($C59 - $D$15)^2 + ($D59 - $E$15)^2)</f>
+        <f t="shared" si="4"/>
         <v>7.8246022263115727</v>
       </c>
       <c r="F59" s="6">
-        <f>SQRT(($C59 - $D$17)^2 + ($D59 - $E$17)^2)</f>
+        <f t="shared" si="5"/>
         <v>17.928798063450881</v>
       </c>
       <c r="G59" s="1">
         <v>2.0099999999999998</v>
       </c>
       <c r="H59" s="6" t="str">
-        <f>IF($F$15-$E59&gt;0,"in range","short")</f>
+        <f t="shared" si="6"/>
         <v>short</v>
       </c>
       <c r="I59" s="2" t="str">
-        <f>IF(B59=$C$15,"Self",IF(B59=$C$17,"Dest",""))</f>
+        <f t="shared" si="7"/>
         <v/>
       </c>
     </row>
@@ -2320,22 +2205,22 @@
         <v>12.47</v>
       </c>
       <c r="E60" s="6">
-        <f>SQRT(($C60 - $D$15)^2 + ($D60 - $E$15)^2)</f>
+        <f t="shared" si="4"/>
         <v>4.0320962290104152</v>
       </c>
       <c r="F60" s="6">
-        <f>SQRT(($C60 - $D$17)^2 + ($D60 - $E$17)^2)</f>
+        <f t="shared" si="5"/>
         <v>11.968976564435239</v>
       </c>
       <c r="G60" s="1">
         <v>5.87</v>
       </c>
       <c r="H60" s="6" t="str">
-        <f>IF($F$15-$E60&gt;0,"in range","short")</f>
+        <f t="shared" si="6"/>
         <v>in range</v>
       </c>
       <c r="I60" s="2" t="str">
-        <f>IF(B60=$C$15,"Self",IF(B60=$C$17,"Dest",""))</f>
+        <f t="shared" si="7"/>
         <v/>
       </c>
     </row>
@@ -2350,22 +2235,22 @@
         <v>14.14</v>
       </c>
       <c r="E61" s="6">
-        <f>SQRT(($C61 - $D$15)^2 + ($D61 - $E$15)^2)</f>
+        <f t="shared" si="4"/>
         <v>5.8831284194720768</v>
       </c>
       <c r="F61" s="6">
-        <f>SQRT(($C61 - $D$17)^2 + ($D61 - $E$17)^2)</f>
+        <f t="shared" si="5"/>
         <v>12.166585387856365</v>
       </c>
       <c r="G61" s="1">
         <v>4.21</v>
       </c>
       <c r="H61" s="6" t="str">
-        <f>IF($F$15-$E61&gt;0,"in range","short")</f>
+        <f t="shared" si="6"/>
         <v>in range</v>
       </c>
       <c r="I61" s="2" t="str">
-        <f>IF(B61=$C$15,"Self",IF(B61=$C$17,"Dest",""))</f>
+        <f t="shared" si="7"/>
         <v/>
       </c>
     </row>
@@ -2380,22 +2265,22 @@
         <v>8.6999999999999993</v>
       </c>
       <c r="E62" s="6">
-        <f>SQRT(($C62 - $D$15)^2 + ($D62 - $E$15)^2)</f>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="F62" s="6">
-        <f>SQRT(($C62 - $D$17)^2 + ($D62 - $E$17)^2)</f>
+        <f t="shared" si="5"/>
         <v>12.854143300897187</v>
       </c>
       <c r="G62" s="1">
         <v>7.49</v>
       </c>
       <c r="H62" s="6" t="str">
-        <f>IF($F$15-$E62&gt;0,"in range","short")</f>
+        <f t="shared" si="6"/>
         <v>in range</v>
       </c>
       <c r="I62" s="2" t="str">
-        <f>IF(B62=$C$15,"Self",IF(B62=$C$17,"Dest",""))</f>
+        <f t="shared" si="7"/>
         <v>Self</v>
       </c>
     </row>
@@ -2410,22 +2295,22 @@
         <v>10.1</v>
       </c>
       <c r="E63" s="6">
-        <f>SQRT(($C63 - $D$15)^2 + ($D63 - $E$15)^2)</f>
+        <f t="shared" si="4"/>
         <v>2.2489108474992956</v>
       </c>
       <c r="F63" s="6">
-        <f>SQRT(($C63 - $D$17)^2 + ($D63 - $E$17)^2)</f>
+        <f t="shared" si="5"/>
         <v>13.3946033909183</v>
       </c>
       <c r="G63" s="1">
         <v>7.25</v>
       </c>
       <c r="H63" s="6" t="str">
-        <f>IF($F$15-$E63&gt;0,"in range","short")</f>
+        <f t="shared" si="6"/>
         <v>in range</v>
       </c>
       <c r="I63" s="2" t="str">
-        <f>IF(B63=$C$15,"Self",IF(B63=$C$17,"Dest",""))</f>
+        <f t="shared" si="7"/>
         <v/>
       </c>
     </row>
@@ -2440,22 +2325,22 @@
         <v>10</v>
       </c>
       <c r="E64" s="6">
-        <f>SQRT(($C64 - $D$15)^2 + ($D64 - $E$15)^2)</f>
+        <f t="shared" si="4"/>
         <v>9.5885348202944947</v>
       </c>
       <c r="F64" s="6">
-        <f>SQRT(($C64 - $D$17)^2 + ($D64 - $E$17)^2)</f>
+        <f t="shared" si="5"/>
         <v>20.370002454589933</v>
       </c>
       <c r="G64" s="1">
         <v>6.31</v>
       </c>
       <c r="H64" s="6" t="str">
-        <f>IF($F$15-$E64&gt;0,"in range","short")</f>
+        <f t="shared" si="6"/>
         <v>short</v>
       </c>
       <c r="I64" s="2" t="str">
-        <f>IF(B64=$C$15,"Self",IF(B64=$C$17,"Dest",""))</f>
+        <f t="shared" si="7"/>
         <v/>
       </c>
     </row>
@@ -2470,22 +2355,22 @@
         <v>5.53</v>
       </c>
       <c r="E65" s="6">
-        <f>SQRT(($C65 - $D$15)^2 + ($D65 - $E$15)^2)</f>
+        <f t="shared" si="4"/>
         <v>4.4408332551448044</v>
       </c>
       <c r="F65" s="6">
-        <f>SQRT(($C65 - $D$17)^2 + ($D65 - $E$17)^2)</f>
+        <f t="shared" si="5"/>
         <v>13.449535307957669</v>
       </c>
       <c r="G65" s="1">
         <v>4.4400000000000004</v>
       </c>
       <c r="H65" s="6" t="str">
-        <f>IF($F$15-$E65&gt;0,"in range","short")</f>
+        <f t="shared" si="6"/>
         <v>in range</v>
       </c>
       <c r="I65" s="2" t="str">
-        <f>IF(B65=$C$15,"Self",IF(B65=$C$17,"Dest",""))</f>
+        <f t="shared" si="7"/>
         <v/>
       </c>
     </row>
@@ -2500,22 +2385,22 @@
         <v>12.85</v>
       </c>
       <c r="E66" s="6">
-        <f>SQRT(($C66 - $D$15)^2 + ($D66 - $E$15)^2)</f>
+        <f t="shared" si="4"/>
         <v>5.4095656017835658</v>
       </c>
       <c r="F66" s="6">
-        <f>SQRT(($C66 - $D$17)^2 + ($D66 - $E$17)^2)</f>
+        <f t="shared" si="5"/>
         <v>13.72559652619878</v>
       </c>
       <c r="G66" s="1">
         <v>4.45</v>
       </c>
       <c r="H66" s="6" t="str">
-        <f>IF($F$15-$E66&gt;0,"in range","short")</f>
+        <f t="shared" si="6"/>
         <v>in range</v>
       </c>
       <c r="I66" s="2" t="str">
-        <f>IF(B66=$C$15,"Self",IF(B66=$C$17,"Dest",""))</f>
+        <f t="shared" si="7"/>
         <v/>
       </c>
     </row>
@@ -2530,22 +2415,22 @@
         <v>8.31</v>
       </c>
       <c r="E67" s="6">
-        <f>SQRT(($C67 - $D$15)^2 + ($D67 - $E$15)^2)</f>
+        <f t="shared" si="4"/>
         <v>1.1576700738984309</v>
       </c>
       <c r="F67" s="6">
-        <f>SQRT(($C67 - $D$17)^2 + ($D67 - $E$17)^2)</f>
+        <f t="shared" si="5"/>
         <v>13.929106216839616</v>
       </c>
       <c r="G67" s="1">
         <v>3.54</v>
       </c>
       <c r="H67" s="6" t="str">
-        <f>IF($F$15-$E67&gt;0,"in range","short")</f>
+        <f t="shared" si="6"/>
         <v>in range</v>
       </c>
       <c r="I67" s="2" t="str">
-        <f>IF(B67=$C$15,"Self",IF(B67=$C$17,"Dest",""))</f>
+        <f t="shared" si="7"/>
         <v/>
       </c>
     </row>
@@ -2560,22 +2445,22 @@
         <v>4.34</v>
       </c>
       <c r="E68" s="6">
-        <f>SQRT(($C68 - $D$15)^2 + ($D68 - $E$15)^2)</f>
+        <f t="shared" si="4"/>
         <v>6.0817102857666612</v>
       </c>
       <c r="F68" s="6">
-        <f>SQRT(($C68 - $D$17)^2 + ($D68 - $E$17)^2)</f>
+        <f t="shared" si="5"/>
         <v>14.047896639710872</v>
       </c>
       <c r="G68" s="1">
         <v>7.78</v>
       </c>
       <c r="H68" s="6" t="str">
-        <f>IF($F$15-$E68&gt;0,"in range","short")</f>
+        <f t="shared" si="6"/>
         <v>in range</v>
       </c>
       <c r="I68" s="2" t="str">
-        <f>IF(B68=$C$15,"Self",IF(B68=$C$17,"Dest",""))</f>
+        <f t="shared" si="7"/>
         <v/>
       </c>
     </row>
@@ -2590,22 +2475,22 @@
         <v>19.36</v>
       </c>
       <c r="E69" s="6">
-        <f>SQRT(($C69 - $D$15)^2 + ($D69 - $E$15)^2)</f>
+        <f t="shared" si="4"/>
         <v>10.667881701631304</v>
       </c>
       <c r="F69" s="6">
-        <f>SQRT(($C69 - $D$17)^2 + ($D69 - $E$17)^2)</f>
+        <f t="shared" si="5"/>
         <v>9.2955096686518477</v>
       </c>
       <c r="G69" s="1">
         <v>4.9400000000000004</v>
       </c>
       <c r="H69" s="6" t="str">
-        <f>IF($F$15-$E69&gt;0,"in range","short")</f>
+        <f t="shared" si="6"/>
         <v>short</v>
       </c>
       <c r="I69" s="2" t="str">
-        <f>IF(B69=$C$15,"Self",IF(B69=$C$17,"Dest",""))</f>
+        <f t="shared" si="7"/>
         <v/>
       </c>
     </row>
@@ -2620,22 +2505,22 @@
         <v>11.33</v>
       </c>
       <c r="E70" s="6">
-        <f>SQRT(($C70 - $D$15)^2 + ($D70 - $E$15)^2)</f>
+        <f t="shared" si="4"/>
         <v>4.7955187414918941</v>
       </c>
       <c r="F70" s="6">
-        <f>SQRT(($C70 - $D$17)^2 + ($D70 - $E$17)^2)</f>
+        <f t="shared" si="5"/>
         <v>14.789577411136534</v>
       </c>
       <c r="G70" s="1">
         <v>1.33</v>
       </c>
       <c r="H70" s="6" t="str">
-        <f>IF($F$15-$E70&gt;0,"in range","short")</f>
+        <f t="shared" si="6"/>
         <v>in range</v>
       </c>
       <c r="I70" s="2" t="str">
-        <f>IF(B70=$C$15,"Self",IF(B70=$C$17,"Dest",""))</f>
+        <f t="shared" si="7"/>
         <v/>
       </c>
     </row>
@@ -2650,22 +2535,22 @@
         <v>13.2</v>
       </c>
       <c r="E71" s="6">
-        <f>SQRT(($C71 - $D$15)^2 + ($D71 - $E$15)^2)</f>
+        <f t="shared" si="4"/>
         <v>6.682334921268164</v>
       </c>
       <c r="F71" s="6">
-        <f>SQRT(($C71 - $D$17)^2 + ($D71 - $E$17)^2)</f>
+        <f t="shared" si="5"/>
         <v>15.020446065280485</v>
       </c>
       <c r="G71" s="1">
         <v>6.76</v>
       </c>
       <c r="H71" s="6" t="str">
-        <f>IF($F$15-$E71&gt;0,"in range","short")</f>
+        <f t="shared" si="6"/>
         <v>in range</v>
       </c>
       <c r="I71" s="2" t="str">
-        <f>IF(B71=$C$15,"Self",IF(B71=$C$17,"Dest",""))</f>
+        <f t="shared" si="7"/>
         <v/>
       </c>
     </row>
@@ -2680,22 +2565,22 @@
         <v>0.02</v>
       </c>
       <c r="E72" s="6">
-        <f>SQRT(($C72 - $D$15)^2 + ($D72 - $E$15)^2)</f>
+        <f t="shared" si="4"/>
         <v>8.6845149547916609</v>
       </c>
       <c r="F72" s="6">
-        <f>SQRT(($C72 - $D$17)^2 + ($D72 - $E$17)^2)</f>
+        <f t="shared" si="5"/>
         <v>19.642978389236191</v>
       </c>
       <c r="G72" s="1">
         <v>2.74</v>
       </c>
       <c r="H72" s="6" t="str">
-        <f>IF($F$15-$E72&gt;0,"in range","short")</f>
+        <f t="shared" si="6"/>
         <v>short</v>
       </c>
       <c r="I72" s="2" t="str">
-        <f>IF(B72=$C$15,"Self",IF(B72=$C$17,"Dest",""))</f>
+        <f t="shared" si="7"/>
         <v/>
       </c>
     </row>
@@ -2710,22 +2595,22 @@
         <v>6.95</v>
       </c>
       <c r="E73" s="6">
-        <f>SQRT(($C73 - $D$15)^2 + ($D73 - $E$15)^2)</f>
+        <f t="shared" si="4"/>
         <v>7.565190017441731</v>
       </c>
       <c r="F73" s="6">
-        <f>SQRT(($C73 - $D$17)^2 + ($D73 - $E$17)^2)</f>
+        <f t="shared" si="5"/>
         <v>19.811584994643919</v>
       </c>
       <c r="G73" s="1">
         <v>3.99</v>
       </c>
       <c r="H73" s="6" t="str">
-        <f>IF($F$15-$E73&gt;0,"in range","short")</f>
+        <f t="shared" si="6"/>
         <v>short</v>
       </c>
       <c r="I73" s="2" t="str">
-        <f>IF(B73=$C$15,"Self",IF(B73=$C$17,"Dest",""))</f>
+        <f t="shared" si="7"/>
         <v/>
       </c>
     </row>
@@ -2740,22 +2625,22 @@
         <v>1.83</v>
       </c>
       <c r="E74" s="6">
-        <f>SQRT(($C74 - $D$15)^2 + ($D74 - $E$15)^2)</f>
+        <f t="shared" si="4"/>
         <v>7.5619111340983105</v>
       </c>
       <c r="F74" s="6">
-        <f>SQRT(($C74 - $D$17)^2 + ($D74 - $E$17)^2)</f>
+        <f t="shared" si="5"/>
         <v>20.037816747340514</v>
       </c>
       <c r="G74" s="1">
         <v>7.57</v>
       </c>
       <c r="H74" s="6" t="str">
-        <f>IF($F$15-$E74&gt;0,"in range","short")</f>
+        <f t="shared" si="6"/>
         <v>short</v>
       </c>
       <c r="I74" s="2" t="str">
-        <f>IF(B74=$C$15,"Self",IF(B74=$C$17,"Dest",""))</f>
+        <f t="shared" si="7"/>
         <v/>
       </c>
     </row>
@@ -2770,22 +2655,22 @@
         <v>4.79</v>
       </c>
       <c r="E75" s="6">
-        <f>SQRT(($C75 - $D$15)^2 + ($D75 - $E$15)^2)</f>
+        <f t="shared" si="4"/>
         <v>3.9418396720313211</v>
       </c>
       <c r="F75" s="6">
-        <f>SQRT(($C75 - $D$17)^2 + ($D75 - $E$17)^2)</f>
+        <f t="shared" si="5"/>
         <v>15.462098822604908</v>
       </c>
       <c r="G75" s="1">
         <v>3.71</v>
       </c>
       <c r="H75" s="6" t="str">
-        <f>IF($F$15-$E75&gt;0,"in range","short")</f>
+        <f t="shared" si="6"/>
         <v>in range</v>
       </c>
       <c r="I75" s="2" t="str">
-        <f>IF(B75=$C$15,"Self",IF(B75=$C$17,"Dest",""))</f>
+        <f t="shared" si="7"/>
         <v/>
       </c>
     </row>
@@ -2800,22 +2685,22 @@
         <v>6.55</v>
       </c>
       <c r="E76" s="6">
-        <f>SQRT(($C76 - $D$15)^2 + ($D76 - $E$15)^2)</f>
+        <f t="shared" si="4"/>
         <v>2.6563320575560567</v>
       </c>
       <c r="F76" s="6">
-        <f>SQRT(($C76 - $D$17)^2 + ($D76 - $E$17)^2)</f>
+        <f t="shared" si="5"/>
         <v>15.465280469490361</v>
       </c>
       <c r="G76" s="1">
         <v>1.36</v>
       </c>
       <c r="H76" s="6" t="str">
-        <f>IF($F$15-$E76&gt;0,"in range","short")</f>
+        <f t="shared" si="6"/>
         <v>in range</v>
       </c>
       <c r="I76" s="2" t="str">
-        <f>IF(B76=$C$15,"Self",IF(B76=$C$17,"Dest",""))</f>
+        <f t="shared" si="7"/>
         <v/>
       </c>
     </row>
@@ -2830,22 +2715,22 @@
         <v>4.47</v>
       </c>
       <c r="E77" s="6">
-        <f>SQRT(($C77 - $D$15)^2 + ($D77 - $E$15)^2)</f>
+        <f t="shared" si="4"/>
         <v>4.3288913130269275</v>
       </c>
       <c r="F77" s="6">
-        <f>SQRT(($C77 - $D$17)^2 + ($D77 - $E$17)^2)</f>
+        <f t="shared" si="5"/>
         <v>15.487249594424442</v>
       </c>
       <c r="G77" s="1">
         <v>6.96</v>
       </c>
       <c r="H77" s="6" t="str">
-        <f>IF($F$15-$E77&gt;0,"in range","short")</f>
+        <f t="shared" si="6"/>
         <v>in range</v>
       </c>
       <c r="I77" s="2" t="str">
-        <f>IF(B77=$C$15,"Self",IF(B77=$C$17,"Dest",""))</f>
+        <f t="shared" si="7"/>
         <v/>
       </c>
     </row>
@@ -2860,22 +2745,22 @@
         <v>3.47</v>
       </c>
       <c r="E78" s="6">
-        <f>SQRT(($C78 - $D$15)^2 + ($D78 - $E$15)^2)</f>
+        <f t="shared" si="4"/>
         <v>5.8054543319192504</v>
       </c>
       <c r="F78" s="6">
-        <f>SQRT(($C78 - $D$17)^2 + ($D78 - $E$17)^2)</f>
+        <f t="shared" si="5"/>
         <v>15.549627005172825</v>
       </c>
       <c r="G78" s="1">
         <v>4.75</v>
       </c>
       <c r="H78" s="6" t="str">
-        <f>IF($F$15-$E78&gt;0,"in range","short")</f>
+        <f t="shared" si="6"/>
         <v>in range</v>
       </c>
       <c r="I78" s="2" t="str">
-        <f>IF(B78=$C$15,"Self",IF(B78=$C$17,"Dest",""))</f>
+        <f t="shared" si="7"/>
         <v/>
       </c>
     </row>
@@ -2890,22 +2775,22 @@
         <v>17.32</v>
       </c>
       <c r="E79" s="6">
-        <f>SQRT(($C79 - $D$15)^2 + ($D79 - $E$15)^2)</f>
+        <f t="shared" si="4"/>
         <v>8.672191187929382</v>
       </c>
       <c r="F79" s="6">
-        <f>SQRT(($C79 - $D$17)^2 + ($D79 - $E$17)^2)</f>
+        <f t="shared" si="5"/>
         <v>10.440119731114198</v>
       </c>
       <c r="G79" s="1">
         <v>5.77</v>
       </c>
       <c r="H79" s="6" t="str">
-        <f>IF($F$15-$E79&gt;0,"in range","short")</f>
+        <f t="shared" si="6"/>
         <v>short</v>
       </c>
       <c r="I79" s="2" t="str">
-        <f>IF(B79=$C$15,"Self",IF(B79=$C$17,"Dest",""))</f>
+        <f t="shared" si="7"/>
         <v/>
       </c>
     </row>
@@ -2920,22 +2805,22 @@
         <v>4.75</v>
       </c>
       <c r="E80" s="6">
-        <f>SQRT(($C80 - $D$15)^2 + ($D80 - $E$15)^2)</f>
+        <f t="shared" si="4"/>
         <v>3.9501139224078075</v>
       </c>
       <c r="F80" s="6">
-        <f>SQRT(($C80 - $D$17)^2 + ($D80 - $E$17)^2)</f>
+        <f t="shared" si="5"/>
         <v>15.772000507227991</v>
       </c>
       <c r="G80" s="1">
         <v>7.56</v>
       </c>
       <c r="H80" s="6" t="str">
-        <f>IF($F$15-$E80&gt;0,"in range","short")</f>
+        <f t="shared" si="6"/>
         <v>in range</v>
       </c>
       <c r="I80" s="2" t="str">
-        <f>IF(B80=$C$15,"Self",IF(B80=$C$17,"Dest",""))</f>
+        <f t="shared" si="7"/>
         <v/>
       </c>
     </row>
@@ -2950,22 +2835,22 @@
         <v>10.050000000000001</v>
       </c>
       <c r="E81" s="6">
-        <f>SQRT(($C81 - $D$15)^2 + ($D81 - $E$15)^2)</f>
+        <f t="shared" si="4"/>
         <v>8.8337647693381545</v>
       </c>
       <c r="F81" s="6">
-        <f>SQRT(($C81 - $D$17)^2 + ($D81 - $E$17)^2)</f>
+        <f t="shared" si="5"/>
         <v>19.635447537553098</v>
       </c>
       <c r="G81" s="1">
         <v>6.33</v>
       </c>
       <c r="H81" s="6" t="str">
-        <f>IF($F$15-$E81&gt;0,"in range","short")</f>
+        <f t="shared" si="6"/>
         <v>short</v>
       </c>
       <c r="I81" s="2" t="str">
-        <f>IF(B81=$C$15,"Self",IF(B81=$C$17,"Dest",""))</f>
+        <f t="shared" si="7"/>
         <v/>
       </c>
     </row>
@@ -2980,22 +2865,22 @@
         <v>7.02</v>
       </c>
       <c r="E82" s="6">
-        <f>SQRT(($C82 - $D$15)^2 + ($D82 - $E$15)^2)</f>
+        <f t="shared" si="4"/>
         <v>8.0962213408478405</v>
       </c>
       <c r="F82" s="6">
-        <f>SQRT(($C82 - $D$17)^2 + ($D82 - $E$17)^2)</f>
+        <f t="shared" si="5"/>
         <v>20.254150191997688</v>
       </c>
       <c r="G82" s="1">
         <v>1.45</v>
       </c>
       <c r="H82" s="6" t="str">
-        <f>IF($F$15-$E82&gt;0,"in range","short")</f>
+        <f t="shared" si="6"/>
         <v>short</v>
       </c>
       <c r="I82" s="2" t="str">
-        <f>IF(B82=$C$15,"Self",IF(B82=$C$17,"Dest",""))</f>
+        <f t="shared" si="7"/>
         <v/>
       </c>
     </row>
@@ -3010,22 +2895,22 @@
         <v>2.52</v>
       </c>
       <c r="E83" s="6">
-        <f>SQRT(($C83 - $D$15)^2 + ($D83 - $E$15)^2)</f>
+        <f t="shared" si="4"/>
         <v>7.6980841772482584</v>
       </c>
       <c r="F83" s="6">
-        <f>SQRT(($C83 - $D$17)^2 + ($D83 - $E$17)^2)</f>
+        <f t="shared" si="5"/>
         <v>20.463843724970147</v>
       </c>
       <c r="G83" s="1">
         <v>7.97</v>
       </c>
       <c r="H83" s="6" t="str">
-        <f>IF($F$15-$E83&gt;0,"in range","short")</f>
+        <f t="shared" si="6"/>
         <v>short</v>
       </c>
       <c r="I83" s="2" t="str">
-        <f>IF(B83=$C$15,"Self",IF(B83=$C$17,"Dest",""))</f>
+        <f t="shared" si="7"/>
         <v/>
       </c>
     </row>
@@ -3040,22 +2925,22 @@
         <v>9.59</v>
       </c>
       <c r="E84" s="6">
-        <f>SQRT(($C84 - $D$15)^2 + ($D84 - $E$15)^2)</f>
+        <f t="shared" ref="E84:E110" si="8">SQRT(($C84 - $D$15)^2 + ($D84 - $E$15)^2)</f>
         <v>4.9506565221190604</v>
       </c>
       <c r="F84" s="6">
-        <f>SQRT(($C84 - $D$17)^2 + ($D84 - $E$17)^2)</f>
+        <f t="shared" ref="F84:F110" si="9">SQRT(($C84 - $D$17)^2 + ($D84 - $E$17)^2)</f>
         <v>16.332115600864451</v>
       </c>
       <c r="G84" s="1">
         <v>3</v>
       </c>
       <c r="H84" s="6" t="str">
-        <f>IF($F$15-$E84&gt;0,"in range","short")</f>
+        <f t="shared" ref="H84:H110" si="10">IF($F$15-$E84&gt;0,"in range","short")</f>
         <v>in range</v>
       </c>
       <c r="I84" s="2" t="str">
-        <f>IF(B84=$C$15,"Self",IF(B84=$C$17,"Dest",""))</f>
+        <f t="shared" ref="I84:I110" si="11">IF(B84=$C$15,"Self",IF(B84=$C$17,"Dest",""))</f>
         <v/>
       </c>
     </row>
@@ -3070,22 +2955,22 @@
         <v>2.56</v>
       </c>
       <c r="E85" s="6">
-        <f>SQRT(($C85 - $D$15)^2 + ($D85 - $E$15)^2)</f>
+        <f t="shared" si="8"/>
         <v>8.0202992462875091</v>
       </c>
       <c r="F85" s="6">
-        <f>SQRT(($C85 - $D$17)^2 + ($D85 - $E$17)^2)</f>
+        <f t="shared" si="9"/>
         <v>20.831673000505745</v>
       </c>
       <c r="G85" s="1">
         <v>2.19</v>
       </c>
       <c r="H85" s="6" t="str">
-        <f>IF($F$15-$E85&gt;0,"in range","short")</f>
+        <f t="shared" si="10"/>
         <v>short</v>
       </c>
       <c r="I85" s="2" t="str">
-        <f>IF(B85=$C$15,"Self",IF(B85=$C$17,"Dest",""))</f>
+        <f t="shared" si="11"/>
         <v/>
       </c>
     </row>
@@ -3100,22 +2985,22 @@
         <v>3.25</v>
       </c>
       <c r="E86" s="6">
-        <f>SQRT(($C86 - $D$15)^2 + ($D86 - $E$15)^2)</f>
+        <f t="shared" si="8"/>
         <v>8.1131128427996124</v>
       </c>
       <c r="F86" s="6">
-        <f>SQRT(($C86 - $D$17)^2 + ($D86 - $E$17)^2)</f>
+        <f t="shared" si="9"/>
         <v>20.96722203821956</v>
       </c>
       <c r="G86" s="1">
         <v>3.19</v>
       </c>
       <c r="H86" s="6" t="str">
-        <f>IF($F$15-$E86&gt;0,"in range","short")</f>
+        <f t="shared" si="10"/>
         <v>short</v>
       </c>
       <c r="I86" s="2" t="str">
-        <f>IF(B86=$C$15,"Self",IF(B86=$C$17,"Dest",""))</f>
+        <f t="shared" si="11"/>
         <v/>
       </c>
     </row>
@@ -3130,22 +3015,22 @@
         <v>6.87</v>
       </c>
       <c r="E87" s="6">
-        <f>SQRT(($C87 - $D$15)^2 + ($D87 - $E$15)^2)</f>
+        <f t="shared" si="8"/>
         <v>3.5912393403949001</v>
       </c>
       <c r="F87" s="6">
-        <f>SQRT(($C87 - $D$17)^2 + ($D87 - $E$17)^2)</f>
+        <f t="shared" si="9"/>
         <v>16.386164896033481</v>
       </c>
       <c r="G87" s="1">
         <v>2.08</v>
       </c>
       <c r="H87" s="6" t="str">
-        <f>IF($F$15-$E87&gt;0,"in range","short")</f>
+        <f t="shared" si="10"/>
         <v>in range</v>
       </c>
       <c r="I87" s="2" t="str">
-        <f>IF(B87=$C$15,"Self",IF(B87=$C$17,"Dest",""))</f>
+        <f t="shared" si="11"/>
         <v/>
       </c>
     </row>
@@ -3160,22 +3045,22 @@
         <v>7.82</v>
       </c>
       <c r="E88" s="6">
-        <f>SQRT(($C88 - $D$15)^2 + ($D88 - $E$15)^2)</f>
+        <f t="shared" si="8"/>
         <v>4.1347309465066759</v>
       </c>
       <c r="F88" s="6">
-        <f>SQRT(($C88 - $D$17)^2 + ($D88 - $E$17)^2)</f>
+        <f t="shared" si="9"/>
         <v>16.56089973401204</v>
       </c>
       <c r="G88" s="1">
         <v>3.56</v>
       </c>
       <c r="H88" s="6" t="str">
-        <f>IF($F$15-$E88&gt;0,"in range","short")</f>
+        <f t="shared" si="10"/>
         <v>in range</v>
       </c>
       <c r="I88" s="2" t="str">
-        <f>IF(B88=$C$15,"Self",IF(B88=$C$17,"Dest",""))</f>
+        <f t="shared" si="11"/>
         <v/>
       </c>
     </row>
@@ -3190,22 +3075,22 @@
         <v>11.61</v>
       </c>
       <c r="E89" s="6">
-        <f>SQRT(($C89 - $D$15)^2 + ($D89 - $E$15)^2)</f>
+        <f t="shared" si="8"/>
         <v>6.80371957094059</v>
       </c>
       <c r="F89" s="6">
-        <f>SQRT(($C89 - $D$17)^2 + ($D89 - $E$17)^2)</f>
+        <f t="shared" si="9"/>
         <v>16.666949330936362</v>
       </c>
       <c r="G89" s="1">
         <v>1.65</v>
       </c>
       <c r="H89" s="6" t="str">
-        <f>IF($F$15-$E89&gt;0,"in range","short")</f>
+        <f t="shared" si="10"/>
         <v>in range</v>
       </c>
       <c r="I89" s="2" t="str">
-        <f>IF(B89=$C$15,"Self",IF(B89=$C$17,"Dest",""))</f>
+        <f t="shared" si="11"/>
         <v/>
       </c>
     </row>
@@ -3220,22 +3105,22 @@
         <v>3.96</v>
       </c>
       <c r="E90" s="6">
-        <f>SQRT(($C90 - $D$15)^2 + ($D90 - $E$15)^2)</f>
+        <f t="shared" si="8"/>
         <v>8.5868038291322328</v>
       </c>
       <c r="F90" s="6">
-        <f>SQRT(($C90 - $D$17)^2 + ($D90 - $E$17)^2)</f>
+        <f t="shared" si="9"/>
         <v>21.378741777756705</v>
       </c>
       <c r="G90" s="1">
         <v>3.93</v>
       </c>
       <c r="H90" s="6" t="str">
-        <f>IF($F$15-$E90&gt;0,"in range","short")</f>
+        <f t="shared" si="10"/>
         <v>short</v>
       </c>
       <c r="I90" s="2" t="str">
-        <f>IF(B90=$C$15,"Self",IF(B90=$C$17,"Dest",""))</f>
+        <f t="shared" si="11"/>
         <v/>
       </c>
     </row>
@@ -3250,22 +3135,22 @@
         <v>2.96</v>
       </c>
       <c r="E91" s="6">
-        <f>SQRT(($C91 - $D$15)^2 + ($D91 - $E$15)^2)</f>
+        <f t="shared" si="8"/>
         <v>5.7500608692430371</v>
       </c>
       <c r="F91" s="6">
-        <f>SQRT(($C91 - $D$17)^2 + ($D91 - $E$17)^2)</f>
+        <f t="shared" si="9"/>
         <v>17.069581131357619</v>
       </c>
       <c r="G91" s="1">
         <v>3.41</v>
       </c>
       <c r="H91" s="6" t="str">
-        <f>IF($F$15-$E91&gt;0,"in range","short")</f>
+        <f t="shared" si="10"/>
         <v>in range</v>
       </c>
       <c r="I91" s="2" t="str">
-        <f>IF(B91=$C$15,"Self",IF(B91=$C$17,"Dest",""))</f>
+        <f t="shared" si="11"/>
         <v/>
       </c>
     </row>
@@ -3280,22 +3165,22 @@
         <v>0.78</v>
       </c>
       <c r="E92" s="6">
-        <f>SQRT(($C92 - $D$15)^2 + ($D92 - $E$15)^2)</f>
+        <f t="shared" si="8"/>
         <v>9.0024885448413645</v>
       </c>
       <c r="F92" s="6">
-        <f>SQRT(($C92 - $D$17)^2 + ($D92 - $E$17)^2)</f>
+        <f t="shared" si="9"/>
         <v>21.560171613417182</v>
       </c>
       <c r="G92" s="1">
         <v>1.97</v>
       </c>
       <c r="H92" s="6" t="str">
-        <f>IF($F$15-$E92&gt;0,"in range","short")</f>
+        <f t="shared" si="10"/>
         <v>short</v>
       </c>
       <c r="I92" s="2" t="str">
-        <f>IF(B92=$C$15,"Self",IF(B92=$C$17,"Dest",""))</f>
+        <f t="shared" si="11"/>
         <v/>
       </c>
     </row>
@@ -3310,22 +3195,22 @@
         <v>6.03</v>
       </c>
       <c r="E93" s="6">
-        <f>SQRT(($C93 - $D$15)^2 + ($D93 - $E$15)^2)</f>
+        <f t="shared" si="8"/>
         <v>9.3110310922045585</v>
       </c>
       <c r="F93" s="6">
-        <f>SQRT(($C93 - $D$17)^2 + ($D93 - $E$17)^2)</f>
+        <f t="shared" si="9"/>
         <v>21.622296362782564</v>
       </c>
       <c r="G93" s="1">
         <v>4.1399999999999997</v>
       </c>
       <c r="H93" s="6" t="str">
-        <f>IF($F$15-$E93&gt;0,"in range","short")</f>
+        <f t="shared" si="10"/>
         <v>short</v>
       </c>
       <c r="I93" s="2" t="str">
-        <f>IF(B93=$C$15,"Self",IF(B93=$C$17,"Dest",""))</f>
+        <f t="shared" si="11"/>
         <v/>
       </c>
     </row>
@@ -3340,22 +3225,22 @@
         <v>4.9000000000000004</v>
       </c>
       <c r="E94" s="6">
-        <f>SQRT(($C94 - $D$15)^2 + ($D94 - $E$15)^2)</f>
+        <f t="shared" si="8"/>
         <v>4.6327637539594004</v>
       </c>
       <c r="F94" s="6">
-        <f>SQRT(($C94 - $D$17)^2 + ($D94 - $E$17)^2)</f>
+        <f t="shared" si="9"/>
         <v>17.403462299209316</v>
       </c>
       <c r="G94" s="1">
         <v>3.58</v>
       </c>
       <c r="H94" s="6" t="str">
-        <f>IF($F$15-$E94&gt;0,"in range","short")</f>
+        <f t="shared" si="10"/>
         <v>in range</v>
       </c>
       <c r="I94" s="2" t="str">
-        <f>IF(B94=$C$15,"Self",IF(B94=$C$17,"Dest",""))</f>
+        <f t="shared" si="11"/>
         <v/>
       </c>
     </row>
@@ -3370,22 +3255,22 @@
         <v>10.92</v>
       </c>
       <c r="E95" s="6">
-        <f>SQRT(($C95 - $D$15)^2 + ($D95 - $E$15)^2)</f>
+        <f t="shared" si="8"/>
         <v>8.5338150905676411</v>
       </c>
       <c r="F95" s="6">
-        <f>SQRT(($C95 - $D$17)^2 + ($D95 - $E$17)^2)</f>
+        <f t="shared" si="9"/>
         <v>18.866780329457384</v>
       </c>
       <c r="G95" s="1">
         <v>3.57</v>
       </c>
       <c r="H95" s="6" t="str">
-        <f>IF($F$15-$E95&gt;0,"in range","short")</f>
+        <f t="shared" si="10"/>
         <v>short</v>
       </c>
       <c r="I95" s="2" t="str">
-        <f>IF(B95=$C$15,"Self",IF(B95=$C$17,"Dest",""))</f>
+        <f t="shared" si="11"/>
         <v/>
       </c>
     </row>
@@ -3400,22 +3285,22 @@
         <v>7.58</v>
       </c>
       <c r="E96" s="6">
-        <f>SQRT(($C96 - $D$15)^2 + ($D96 - $E$15)^2)</f>
+        <f t="shared" si="8"/>
         <v>8.9701950926387326</v>
       </c>
       <c r="F96" s="6">
-        <f>SQRT(($C96 - $D$17)^2 + ($D96 - $E$17)^2)</f>
+        <f t="shared" si="9"/>
         <v>9.8077622320282636</v>
       </c>
       <c r="G96" s="1">
         <v>2.44</v>
       </c>
       <c r="H96" s="6" t="str">
-        <f>IF($F$15-$E96&gt;0,"in range","short")</f>
+        <f t="shared" si="10"/>
         <v>short</v>
       </c>
       <c r="I96" s="2" t="str">
-        <f>IF(B96=$C$15,"Self",IF(B96=$C$17,"Dest",""))</f>
+        <f t="shared" si="11"/>
         <v/>
       </c>
     </row>
@@ -3430,22 +3315,22 @@
         <v>2.29</v>
       </c>
       <c r="E97" s="6">
-        <f>SQRT(($C97 - $D$15)^2 + ($D97 - $E$15)^2)</f>
+        <f t="shared" si="8"/>
         <v>8.5248167135722035</v>
       </c>
       <c r="F97" s="6">
-        <f>SQRT(($C97 - $D$17)^2 + ($D97 - $E$17)^2)</f>
+        <f t="shared" si="9"/>
         <v>15.568664040308663</v>
       </c>
       <c r="G97" s="1">
         <v>2.5</v>
       </c>
       <c r="H97" s="6" t="str">
-        <f>IF($F$15-$E97&gt;0,"in range","short")</f>
+        <f t="shared" si="10"/>
         <v>short</v>
       </c>
       <c r="I97" s="2" t="str">
-        <f>IF(B97=$C$15,"Self",IF(B97=$C$17,"Dest",""))</f>
+        <f t="shared" si="11"/>
         <v/>
       </c>
     </row>
@@ -3460,22 +3345,22 @@
         <v>7.45</v>
       </c>
       <c r="E98" s="6">
-        <f>SQRT(($C98 - $D$15)^2 + ($D98 - $E$15)^2)</f>
+        <f t="shared" si="8"/>
         <v>9.2151722718568863</v>
       </c>
       <c r="F98" s="6">
-        <f>SQRT(($C98 - $D$17)^2 + ($D98 - $E$17)^2)</f>
+        <f t="shared" si="9"/>
         <v>9.926530108754017</v>
       </c>
       <c r="G98" s="1">
         <v>2.4300000000000002</v>
       </c>
       <c r="H98" s="6" t="str">
-        <f>IF($F$15-$E98&gt;0,"in range","short")</f>
+        <f t="shared" si="10"/>
         <v>short</v>
       </c>
       <c r="I98" s="2" t="str">
-        <f>IF(B98=$C$15,"Self",IF(B98=$C$17,"Dest",""))</f>
+        <f t="shared" si="11"/>
         <v/>
       </c>
     </row>
@@ -3490,22 +3375,22 @@
         <v>4.3899999999999997</v>
       </c>
       <c r="E99" s="6">
-        <f>SQRT(($C99 - $D$15)^2 + ($D99 - $E$15)^2)</f>
+        <f t="shared" si="8"/>
         <v>8.3657037958560299</v>
       </c>
       <c r="F99" s="6">
-        <f>SQRT(($C99 - $D$17)^2 + ($D99 - $E$17)^2)</f>
+        <f t="shared" si="9"/>
         <v>13.185704380123195</v>
       </c>
       <c r="G99" s="1">
         <v>1.18</v>
       </c>
       <c r="H99" s="6" t="str">
-        <f>IF($F$15-$E99&gt;0,"in range","short")</f>
+        <f t="shared" si="10"/>
         <v>short</v>
       </c>
       <c r="I99" s="2" t="str">
-        <f>IF(B99=$C$15,"Self",IF(B99=$C$17,"Dest",""))</f>
+        <f t="shared" si="11"/>
         <v/>
       </c>
     </row>
@@ -3520,22 +3405,22 @@
         <v>4.05</v>
       </c>
       <c r="E100" s="6">
-        <f>SQRT(($C100 - $D$15)^2 + ($D100 - $E$15)^2)</f>
+        <f t="shared" si="8"/>
         <v>5.3324103367989224</v>
       </c>
       <c r="F100" s="6">
-        <f>SQRT(($C100 - $D$17)^2 + ($D100 - $E$17)^2)</f>
+        <f t="shared" si="9"/>
         <v>17.995343842227634</v>
       </c>
       <c r="G100" s="1">
         <v>6.92</v>
       </c>
       <c r="H100" s="6" t="str">
-        <f>IF($F$15-$E100&gt;0,"in range","short")</f>
+        <f t="shared" si="10"/>
         <v>in range</v>
       </c>
       <c r="I100" s="2" t="str">
-        <f>IF(B100=$C$15,"Self",IF(B100=$C$17,"Dest",""))</f>
+        <f t="shared" si="11"/>
         <v/>
       </c>
     </row>
@@ -3550,22 +3435,22 @@
         <v>4.7</v>
       </c>
       <c r="E101" s="6">
-        <f>SQRT(($C101 - $D$15)^2 + ($D101 - $E$15)^2)</f>
+        <f t="shared" si="8"/>
         <v>9.29473506884408</v>
       </c>
       <c r="F101" s="6">
-        <f>SQRT(($C101 - $D$17)^2 + ($D101 - $E$17)^2)</f>
+        <f t="shared" si="9"/>
         <v>21.91399780961931</v>
       </c>
       <c r="G101" s="1">
         <v>3.25</v>
       </c>
       <c r="H101" s="6" t="str">
-        <f>IF($F$15-$E101&gt;0,"in range","short")</f>
+        <f t="shared" si="10"/>
         <v>short</v>
       </c>
       <c r="I101" s="2" t="str">
-        <f>IF(B101=$C$15,"Self",IF(B101=$C$17,"Dest",""))</f>
+        <f t="shared" si="11"/>
         <v/>
       </c>
     </row>
@@ -3580,22 +3465,22 @@
         <v>3.32</v>
       </c>
       <c r="E102" s="6">
-        <f>SQRT(($C102 - $D$15)^2 + ($D102 - $E$15)^2)</f>
+        <f t="shared" si="8"/>
         <v>5.7259060418417613</v>
       </c>
       <c r="F102" s="6">
-        <f>SQRT(($C102 - $D$17)^2 + ($D102 - $E$17)^2)</f>
+        <f t="shared" si="9"/>
         <v>18.124706894181763</v>
       </c>
       <c r="G102" s="1">
         <v>6.81</v>
       </c>
       <c r="H102" s="6" t="str">
-        <f>IF($F$15-$E102&gt;0,"in range","short")</f>
+        <f t="shared" si="10"/>
         <v>in range</v>
       </c>
       <c r="I102" s="2" t="str">
-        <f>IF(B102=$C$15,"Self",IF(B102=$C$17,"Dest",""))</f>
+        <f t="shared" si="11"/>
         <v/>
       </c>
     </row>
@@ -3610,22 +3495,22 @@
         <v>2.15</v>
       </c>
       <c r="E103" s="6">
-        <f>SQRT(($C103 - $D$15)^2 + ($D103 - $E$15)^2)</f>
+        <f t="shared" si="8"/>
         <v>11.309770112606179</v>
       </c>
       <c r="F103" s="6">
-        <f>SQRT(($C103 - $D$17)^2 + ($D103 - $E$17)^2)</f>
+        <f t="shared" si="9"/>
         <v>15.222394686776454</v>
       </c>
       <c r="G103" s="1">
         <v>1.99</v>
       </c>
       <c r="H103" s="6" t="str">
-        <f>IF($F$15-$E103&gt;0,"in range","short")</f>
+        <f t="shared" si="10"/>
         <v>short</v>
       </c>
       <c r="I103" s="2" t="str">
-        <f>IF(B103=$C$15,"Self",IF(B103=$C$17,"Dest",""))</f>
+        <f t="shared" si="11"/>
         <v/>
       </c>
     </row>
@@ -3640,22 +3525,22 @@
         <v>5.63</v>
       </c>
       <c r="E104" s="6">
-        <f>SQRT(($C104 - $D$15)^2 + ($D104 - $E$15)^2)</f>
+        <f t="shared" si="8"/>
         <v>10.326882394992209</v>
       </c>
       <c r="F104" s="6">
-        <f>SQRT(($C104 - $D$17)^2 + ($D104 - $E$17)^2)</f>
+        <f t="shared" si="9"/>
         <v>11.74582904694258</v>
       </c>
       <c r="G104" s="1">
         <v>1.31</v>
       </c>
       <c r="H104" s="6" t="str">
-        <f>IF($F$15-$E104&gt;0,"in range","short")</f>
+        <f t="shared" si="10"/>
         <v>short</v>
       </c>
       <c r="I104" s="2" t="str">
-        <f>IF(B104=$C$15,"Self",IF(B104=$C$17,"Dest",""))</f>
+        <f t="shared" si="11"/>
         <v/>
       </c>
     </row>
@@ -3670,22 +3555,22 @@
         <v>2.99</v>
       </c>
       <c r="E105" s="6">
-        <f>SQRT(($C105 - $D$15)^2 + ($D105 - $E$15)^2)</f>
+        <f t="shared" si="8"/>
         <v>5.9492016271093036</v>
       </c>
       <c r="F105" s="6">
-        <f>SQRT(($C105 - $D$17)^2 + ($D105 - $E$17)^2)</f>
+        <f t="shared" si="9"/>
         <v>18.202472359545009</v>
       </c>
       <c r="G105" s="1">
         <v>6.34</v>
       </c>
       <c r="H105" s="6" t="str">
-        <f>IF($F$15-$E105&gt;0,"in range","short")</f>
+        <f t="shared" si="10"/>
         <v>in range</v>
       </c>
       <c r="I105" s="2" t="str">
-        <f>IF(B105=$C$15,"Self",IF(B105=$C$17,"Dest",""))</f>
+        <f t="shared" si="11"/>
         <v/>
       </c>
     </row>
@@ -3700,22 +3585,22 @@
         <v>1.34</v>
       </c>
       <c r="E106" s="6">
-        <f>SQRT(($C106 - $D$15)^2 + ($D106 - $E$15)^2)</f>
+        <f t="shared" si="8"/>
         <v>9.7534404186420289</v>
       </c>
       <c r="F106" s="6">
-        <f>SQRT(($C106 - $D$17)^2 + ($D106 - $E$17)^2)</f>
+        <f t="shared" si="9"/>
         <v>22.571065548617771</v>
       </c>
       <c r="G106" s="1">
         <v>5.44</v>
       </c>
       <c r="H106" s="6" t="str">
-        <f>IF($F$15-$E106&gt;0,"in range","short")</f>
+        <f t="shared" si="10"/>
         <v>short</v>
       </c>
       <c r="I106" s="2" t="str">
-        <f>IF(B106=$C$15,"Self",IF(B106=$C$17,"Dest",""))</f>
+        <f t="shared" si="11"/>
         <v/>
       </c>
     </row>
@@ -3730,22 +3615,22 @@
         <v>2.9</v>
       </c>
       <c r="E107" s="6">
-        <f>SQRT(($C107 - $D$15)^2 + ($D107 - $E$15)^2)</f>
+        <f t="shared" si="8"/>
         <v>6.0139920186179152</v>
       </c>
       <c r="F107" s="6">
-        <f>SQRT(($C107 - $D$17)^2 + ($D107 - $E$17)^2)</f>
+        <f t="shared" si="9"/>
         <v>18.224908778921229</v>
       </c>
       <c r="G107" s="1">
         <v>5.22</v>
       </c>
       <c r="H107" s="6" t="str">
-        <f>IF($F$15-$E107&gt;0,"in range","short")</f>
+        <f t="shared" si="10"/>
         <v>in range</v>
       </c>
       <c r="I107" s="2" t="str">
-        <f>IF(B107=$C$15,"Self",IF(B107=$C$17,"Dest",""))</f>
+        <f t="shared" si="11"/>
         <v/>
       </c>
     </row>
@@ -3760,22 +3645,22 @@
         <v>4.1500000000000004</v>
       </c>
       <c r="E108" s="6">
-        <f>SQRT(($C108 - $D$15)^2 + ($D108 - $E$15)^2)</f>
+        <f t="shared" si="8"/>
         <v>9.9244596830255674</v>
       </c>
       <c r="F108" s="6">
-        <f>SQRT(($C108 - $D$17)^2 + ($D108 - $E$17)^2)</f>
+        <f t="shared" si="9"/>
         <v>22.583722013875391</v>
       </c>
       <c r="G108" s="1">
         <v>5.1100000000000003</v>
       </c>
       <c r="H108" s="6" t="str">
-        <f>IF($F$15-$E108&gt;0,"in range","short")</f>
+        <f t="shared" si="10"/>
         <v>short</v>
       </c>
       <c r="I108" s="2" t="str">
-        <f>IF(B108=$C$15,"Self",IF(B108=$C$17,"Dest",""))</f>
+        <f t="shared" si="11"/>
         <v/>
       </c>
     </row>
@@ -3790,22 +3675,22 @@
         <v>0.7</v>
       </c>
       <c r="E109" s="6">
-        <f>SQRT(($C109 - $D$15)^2 + ($D109 - $E$15)^2)</f>
+        <f t="shared" si="8"/>
         <v>10.643326547654166</v>
       </c>
       <c r="F109" s="6">
-        <f>SQRT(($C109 - $D$17)^2 + ($D109 - $E$17)^2)</f>
+        <f t="shared" si="9"/>
         <v>23.462075781993374</v>
       </c>
       <c r="G109" s="1">
         <v>5.45</v>
       </c>
       <c r="H109" s="6" t="str">
-        <f>IF($F$15-$E109&gt;0,"in range","short")</f>
+        <f t="shared" si="10"/>
         <v>short</v>
       </c>
       <c r="I109" s="2" t="str">
-        <f>IF(B109=$C$15,"Self",IF(B109=$C$17,"Dest",""))</f>
+        <f t="shared" si="11"/>
         <v/>
       </c>
     </row>
@@ -3820,22 +3705,22 @@
         <v>2.67</v>
       </c>
       <c r="E110" s="6">
-        <f>SQRT(($C110 - $D$15)^2 + ($D110 - $E$15)^2)</f>
+        <f t="shared" si="8"/>
         <v>7.3371179627971088</v>
       </c>
       <c r="F110" s="6">
-        <f>SQRT(($C110 - $D$17)^2 + ($D110 - $E$17)^2)</f>
+        <f t="shared" si="9"/>
         <v>20.073836205369417</v>
       </c>
       <c r="G110" s="1">
         <v>1.38</v>
       </c>
       <c r="H110" s="6" t="str">
-        <f>IF($F$15-$E110&gt;0,"in range","short")</f>
+        <f t="shared" si="10"/>
         <v>in range</v>
       </c>
       <c r="I110" s="2" t="str">
-        <f>IF(B110=$C$15,"Self",IF(B110=$C$17,"Dest",""))</f>
+        <f t="shared" si="11"/>
         <v/>
       </c>
     </row>
@@ -3849,6 +3734,12 @@
     <sortCondition ref="B20:B34"/>
   </sortState>
   <mergeCells count="22">
+    <mergeCell ref="C8:C9"/>
+    <mergeCell ref="C10:C11"/>
+    <mergeCell ref="D4:D5"/>
+    <mergeCell ref="E4:E5"/>
+    <mergeCell ref="D8:D9"/>
+    <mergeCell ref="E8:E9"/>
     <mergeCell ref="D2:G2"/>
     <mergeCell ref="B4:B11"/>
     <mergeCell ref="F8:F9"/>
@@ -3865,29 +3756,213 @@
     <mergeCell ref="G6:G7"/>
     <mergeCell ref="C4:C5"/>
     <mergeCell ref="C6:C7"/>
-    <mergeCell ref="C8:C9"/>
-    <mergeCell ref="C10:C11"/>
-    <mergeCell ref="D4:D5"/>
-    <mergeCell ref="E4:E5"/>
-    <mergeCell ref="D8:D9"/>
-    <mergeCell ref="E8:E9"/>
   </mergeCells>
   <conditionalFormatting sqref="H20:H110">
-    <cfRule type="containsText" dxfId="8" priority="6" stopIfTrue="1" operator="containsText" text="short">
+    <cfRule type="containsText" dxfId="3" priority="6" stopIfTrue="1" operator="containsText" text="short">
       <formula>NOT(ISERROR(SEARCH("short",H20)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="7" priority="7" operator="containsText" text="in range">
+    <cfRule type="containsText" dxfId="2" priority="7" operator="containsText" text="in range">
       <formula>NOT(ISERROR(SEARCH("in range",H20)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I20:I110">
-    <cfRule type="containsText" dxfId="6" priority="5" operator="containsText" text="Self">
+    <cfRule type="containsText" dxfId="1" priority="4" stopIfTrue="1" operator="containsText" text="Dest">
+      <formula>NOT(ISERROR(SEARCH("Dest",I20)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="0" priority="5" operator="containsText" text="Self">
       <formula>NOT(ISERROR(SEARCH("Self",I20)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="5" priority="4" stopIfTrue="1" operator="containsText" text="Dest">
-      <formula>NOT(ISERROR(SEARCH("Dest",I20)))</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{129E912C-5949-4C72-88F1-D72656C04391}">
+  <dimension ref="B2:I10"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="L18" sqref="L18"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="2" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="D2" s="17" t="s">
+        <v>0</v>
+      </c>
+      <c r="E2" s="17" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="C3" t="s">
+        <v>21</v>
+      </c>
+      <c r="D3" s="17">
+        <v>7.5</v>
+      </c>
+      <c r="E3" s="17">
+        <v>7.5</v>
+      </c>
+    </row>
+    <row r="4" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B4" s="17" t="s">
+        <v>0</v>
+      </c>
+      <c r="C4" s="17" t="s">
+        <v>1</v>
+      </c>
+      <c r="D4" s="17" t="s">
+        <v>20</v>
+      </c>
+      <c r="E4" s="17" t="s">
+        <v>19</v>
+      </c>
+      <c r="F4" s="17" t="s">
+        <v>18</v>
+      </c>
+      <c r="G4" s="17" t="s">
+        <v>17</v>
+      </c>
+      <c r="I4" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="5" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B5" s="17">
+        <v>5</v>
+      </c>
+      <c r="C5" s="17">
+        <v>5</v>
+      </c>
+      <c r="D5" s="17">
+        <v>4</v>
+      </c>
+      <c r="E5" s="17">
+        <v>70</v>
+      </c>
+      <c r="F5" s="17">
+        <v>40</v>
+      </c>
+      <c r="G5" s="17">
+        <f>0.4*D5+0.4*E5+0.2*F5</f>
+        <v>37.6</v>
+      </c>
+      <c r="I5">
+        <f>SQRT(($D$3-B5)^2+($E$3-C5)^2)</f>
+        <v>3.5355339059327378</v>
+      </c>
+    </row>
+    <row r="6" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B6" s="17">
+        <v>6</v>
+      </c>
+      <c r="C6" s="17">
+        <v>6</v>
+      </c>
+      <c r="D6" s="17">
+        <v>3</v>
+      </c>
+      <c r="E6" s="17">
+        <v>80</v>
+      </c>
+      <c r="F6" s="17">
+        <v>50</v>
+      </c>
+      <c r="G6" s="17">
+        <f t="shared" ref="G6:G9" si="0">0.4*D6+0.4*E6+0.2*F6</f>
+        <v>43.2</v>
+      </c>
+      <c r="I6">
+        <f>SQRT(($D$3-B6)^2+($E$3-C6)^2)</f>
+        <v>2.1213203435596424</v>
+      </c>
+    </row>
+    <row r="7" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B7" s="17">
+        <v>7</v>
+      </c>
+      <c r="C7" s="17">
+        <v>7</v>
+      </c>
+      <c r="D7" s="17">
+        <v>2</v>
+      </c>
+      <c r="E7" s="17">
+        <v>60</v>
+      </c>
+      <c r="F7" s="17">
+        <v>20</v>
+      </c>
+      <c r="G7" s="17">
+        <f t="shared" si="0"/>
+        <v>28.8</v>
+      </c>
+      <c r="I7">
+        <f>SQRT(($D$3-B7)^2+($E$3-C7)^2)</f>
+        <v>0.70710678118654757</v>
+      </c>
+    </row>
+    <row r="8" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B8" s="17">
+        <v>5</v>
+      </c>
+      <c r="C8" s="17">
+        <v>9</v>
+      </c>
+      <c r="D8" s="17">
+        <v>3</v>
+      </c>
+      <c r="E8" s="17">
+        <v>80</v>
+      </c>
+      <c r="F8" s="17">
+        <v>50</v>
+      </c>
+      <c r="G8" s="17">
+        <f t="shared" si="0"/>
+        <v>43.2</v>
+      </c>
+      <c r="I8">
+        <f>SQRT(($D$3-B8)^2+($E$3-C8)^2)</f>
+        <v>2.9154759474226504</v>
+      </c>
+    </row>
+    <row r="9" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B9" s="17">
+        <v>9</v>
+      </c>
+      <c r="C9" s="17">
+        <v>9</v>
+      </c>
+      <c r="D9" s="17">
+        <v>3</v>
+      </c>
+      <c r="E9" s="17">
+        <v>80</v>
+      </c>
+      <c r="F9" s="17">
+        <v>50</v>
+      </c>
+      <c r="G9" s="17">
+        <f t="shared" si="0"/>
+        <v>43.2</v>
+      </c>
+      <c r="I9">
+        <f>SQRT(($D$3-B9)^2+($E$3-C9)^2)</f>
+        <v>2.1213203435596424</v>
+      </c>
+    </row>
+    <row r="10" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B10" s="17"/>
+      <c r="C10" s="17"/>
+      <c r="D10" s="17"/>
+      <c r="E10" s="17"/>
+      <c r="F10" s="17"/>
+      <c r="G10" s="17"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>